<commit_message>
Regenerated output files after working on a range of tickets related to extensions, json files and CDA-IG pdfs updates
</commit_message>
<xml_diff>
--- a/output/AdvanceCareRecords/patient-dh-base-1.xlsx
+++ b/output/AdvanceCareRecords/patient-dh-base-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6974" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6974" uniqueCount="639">
   <si>
     <t>Path</t>
   </si>
@@ -358,7 +358,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
     <t>indigenousStatus</t>
@@ -1457,10 +1457,6 @@
   </si>
   <si>
     <t>In some circumstances, systems may only have date or datetime data that has unknown or estimated parts.  This coding establishes the acuraccy of the day, month and year parts.</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
     <t>Patient.deceasedDateTime.value</t>
@@ -20043,7 +20039,7 @@
         <v>107</v>
       </c>
       <c r="AI156" t="s" s="2">
-        <v>453</v>
+        <v>108</v>
       </c>
       <c r="AJ156" t="s" s="2">
         <v>44</v>
@@ -20063,7 +20059,7 @@
     </row>
     <row r="157" hidden="true">
       <c r="A157" t="s" s="2">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B157" s="2"/>
       <c r="C157" t="s" s="2">
@@ -20089,7 +20085,7 @@
         <v>427</v>
       </c>
       <c r="K157" t="s" s="2">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="L157" t="s" s="2">
         <v>429</v>
@@ -20143,7 +20139,7 @@
         <v>44</v>
       </c>
       <c r="AE157" t="s" s="2">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="AF157" t="s" s="2">
         <v>42</v>
@@ -20175,7 +20171,7 @@
     </row>
     <row r="158">
       <c r="A158" t="s" s="2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B158" s="2"/>
       <c r="C158" t="s" s="2">
@@ -20198,19 +20194,19 @@
         <v>53</v>
       </c>
       <c r="J158" t="s" s="2">
+        <v>457</v>
+      </c>
+      <c r="K158" t="s" s="2">
         <v>458</v>
       </c>
-      <c r="K158" t="s" s="2">
+      <c r="L158" t="s" s="2">
         <v>459</v>
       </c>
-      <c r="L158" t="s" s="2">
+      <c r="M158" t="s" s="2">
         <v>460</v>
       </c>
-      <c r="M158" t="s" s="2">
+      <c r="N158" t="s" s="2">
         <v>461</v>
-      </c>
-      <c r="N158" t="s" s="2">
-        <v>462</v>
       </c>
       <c r="O158" t="s" s="2">
         <v>44</v>
@@ -20259,7 +20255,7 @@
         <v>44</v>
       </c>
       <c r="AE158" t="s" s="2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AF158" t="s" s="2">
         <v>42</v>
@@ -20274,16 +20270,16 @@
         <v>44</v>
       </c>
       <c r="AJ158" t="s" s="2">
+        <v>462</v>
+      </c>
+      <c r="AK158" t="s" s="2">
         <v>463</v>
       </c>
-      <c r="AK158" t="s" s="2">
+      <c r="AL158" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM158" t="s" s="2">
         <v>464</v>
-      </c>
-      <c r="AL158" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM158" t="s" s="2">
-        <v>465</v>
       </c>
       <c r="AN158" t="s" s="2">
         <v>44</v>
@@ -20291,7 +20287,7 @@
     </row>
     <row r="159">
       <c r="A159" t="s" s="2">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B159" s="2"/>
       <c r="C159" t="s" s="2">
@@ -20317,14 +20313,14 @@
         <v>193</v>
       </c>
       <c r="K159" t="s" s="2">
+        <v>466</v>
+      </c>
+      <c r="L159" t="s" s="2">
         <v>467</v>
-      </c>
-      <c r="L159" t="s" s="2">
-        <v>468</v>
       </c>
       <c r="M159" s="2"/>
       <c r="N159" t="s" s="2">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="O159" t="s" s="2">
         <v>44</v>
@@ -20352,52 +20348,52 @@
         <v>75</v>
       </c>
       <c r="X159" t="s" s="2">
+        <v>469</v>
+      </c>
+      <c r="Y159" t="s" s="2">
         <v>470</v>
       </c>
-      <c r="Y159" t="s" s="2">
+      <c r="Z159" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA159" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB159" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC159" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD159" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE159" t="s" s="2">
+        <v>465</v>
+      </c>
+      <c r="AF159" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG159" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH159" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI159" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ159" t="s" s="2">
         <v>471</v>
       </c>
-      <c r="Z159" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA159" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB159" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC159" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD159" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE159" t="s" s="2">
-        <v>466</v>
-      </c>
-      <c r="AF159" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG159" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH159" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI159" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ159" t="s" s="2">
+      <c r="AK159" t="s" s="2">
         <v>472</v>
       </c>
-      <c r="AK159" t="s" s="2">
+      <c r="AL159" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM159" t="s" s="2">
         <v>473</v>
-      </c>
-      <c r="AL159" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM159" t="s" s="2">
-        <v>474</v>
       </c>
       <c r="AN159" t="s" s="2">
         <v>44</v>
@@ -20405,7 +20401,7 @@
     </row>
     <row r="160">
       <c r="A160" t="s" s="2">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B160" s="2"/>
       <c r="C160" t="s" s="2">
@@ -20428,19 +20424,19 @@
         <v>44</v>
       </c>
       <c r="J160" t="s" s="2">
+        <v>475</v>
+      </c>
+      <c r="K160" t="s" s="2">
         <v>476</v>
       </c>
-      <c r="K160" t="s" s="2">
+      <c r="L160" t="s" s="2">
         <v>477</v>
       </c>
-      <c r="L160" t="s" s="2">
+      <c r="M160" t="s" s="2">
         <v>478</v>
       </c>
-      <c r="M160" t="s" s="2">
+      <c r="N160" t="s" s="2">
         <v>479</v>
-      </c>
-      <c r="N160" t="s" s="2">
-        <v>480</v>
       </c>
       <c r="O160" t="s" s="2">
         <v>44</v>
@@ -20489,7 +20485,7 @@
         <v>44</v>
       </c>
       <c r="AE160" t="s" s="2">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="AF160" t="s" s="2">
         <v>42</v>
@@ -20504,7 +20500,7 @@
         <v>44</v>
       </c>
       <c r="AJ160" t="s" s="2">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="AK160" t="s" s="2">
         <v>148</v>
@@ -20513,7 +20509,7 @@
         <v>44</v>
       </c>
       <c r="AM160" t="s" s="2">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AN160" t="s" s="2">
         <v>44</v>
@@ -20521,7 +20517,7 @@
     </row>
     <row r="161">
       <c r="A161" t="s" s="2">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B161" s="2"/>
       <c r="C161" t="s" s="2">
@@ -20544,17 +20540,17 @@
         <v>44</v>
       </c>
       <c r="J161" t="s" s="2">
+        <v>483</v>
+      </c>
+      <c r="K161" t="s" s="2">
         <v>484</v>
       </c>
-      <c r="K161" t="s" s="2">
+      <c r="L161" t="s" s="2">
         <v>485</v>
-      </c>
-      <c r="L161" t="s" s="2">
-        <v>486</v>
       </c>
       <c r="M161" s="2"/>
       <c r="N161" t="s" s="2">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O161" t="s" s="2">
         <v>44</v>
@@ -20603,7 +20599,7 @@
         <v>44</v>
       </c>
       <c r="AE161" t="s" s="2">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="AF161" t="s" s="2">
         <v>42</v>
@@ -20618,7 +20614,7 @@
         <v>44</v>
       </c>
       <c r="AJ161" t="s" s="2">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="AK161" t="s" s="2">
         <v>148</v>
@@ -20627,7 +20623,7 @@
         <v>44</v>
       </c>
       <c r="AM161" t="s" s="2">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="AN161" t="s" s="2">
         <v>44</v>
@@ -20635,7 +20631,7 @@
     </row>
     <row r="162">
       <c r="A162" t="s" s="2">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" t="s" s="2">
@@ -20658,19 +20654,19 @@
         <v>44</v>
       </c>
       <c r="J162" t="s" s="2">
+        <v>490</v>
+      </c>
+      <c r="K162" t="s" s="2">
         <v>491</v>
       </c>
-      <c r="K162" t="s" s="2">
+      <c r="L162" t="s" s="2">
         <v>492</v>
       </c>
-      <c r="L162" t="s" s="2">
+      <c r="M162" t="s" s="2">
         <v>493</v>
       </c>
-      <c r="M162" t="s" s="2">
+      <c r="N162" t="s" s="2">
         <v>494</v>
-      </c>
-      <c r="N162" t="s" s="2">
-        <v>495</v>
       </c>
       <c r="O162" t="s" s="2">
         <v>44</v>
@@ -20719,7 +20715,7 @@
         <v>44</v>
       </c>
       <c r="AE162" t="s" s="2">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="AF162" t="s" s="2">
         <v>42</v>
@@ -20731,10 +20727,10 @@
         <v>44</v>
       </c>
       <c r="AI162" t="s" s="2">
+        <v>495</v>
+      </c>
+      <c r="AJ162" t="s" s="2">
         <v>496</v>
-      </c>
-      <c r="AJ162" t="s" s="2">
-        <v>497</v>
       </c>
       <c r="AK162" t="s" s="2">
         <v>148</v>
@@ -20751,7 +20747,7 @@
     </row>
     <row r="163" hidden="true">
       <c r="A163" t="s" s="2">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" t="s" s="2">
@@ -20863,7 +20859,7 @@
     </row>
     <row r="164" hidden="true">
       <c r="A164" t="s" s="2">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B164" s="2"/>
       <c r="C164" t="s" s="2">
@@ -20977,11 +20973,11 @@
     </row>
     <row r="165" hidden="true">
       <c r="A165" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B165" s="2"/>
       <c r="C165" t="s" s="2">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D165" s="2"/>
       <c r="E165" t="s" s="2">
@@ -21006,7 +21002,7 @@
         <v>125</v>
       </c>
       <c r="L165" t="s" s="2">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="M165" t="s" s="2">
         <v>127</v>
@@ -21059,7 +21055,7 @@
         <v>44</v>
       </c>
       <c r="AE165" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="AF165" t="s" s="2">
         <v>42</v>
@@ -21091,7 +21087,7 @@
     </row>
     <row r="166">
       <c r="A166" t="s" s="2">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B166" s="2"/>
       <c r="C166" t="s" s="2">
@@ -21117,14 +21113,14 @@
         <v>193</v>
       </c>
       <c r="K166" t="s" s="2">
+        <v>504</v>
+      </c>
+      <c r="L166" t="s" s="2">
         <v>505</v>
-      </c>
-      <c r="L166" t="s" s="2">
-        <v>506</v>
       </c>
       <c r="M166" s="2"/>
       <c r="N166" t="s" s="2">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="O166" t="s" s="2">
         <v>44</v>
@@ -21153,7 +21149,7 @@
       </c>
       <c r="X166" s="2"/>
       <c r="Y166" t="s" s="2">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Z166" t="s" s="2">
         <v>44</v>
@@ -21171,7 +21167,7 @@
         <v>44</v>
       </c>
       <c r="AE166" t="s" s="2">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="AF166" t="s" s="2">
         <v>42</v>
@@ -21186,7 +21182,7 @@
         <v>44</v>
       </c>
       <c r="AJ166" t="s" s="2">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AK166" t="s" s="2">
         <v>148</v>
@@ -21195,7 +21191,7 @@
         <v>44</v>
       </c>
       <c r="AM166" t="s" s="2">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="AN166" t="s" s="2">
         <v>44</v>
@@ -21203,7 +21199,7 @@
     </row>
     <row r="167">
       <c r="A167" t="s" s="2">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B167" s="2"/>
       <c r="C167" t="s" s="2">
@@ -21229,14 +21225,14 @@
         <v>376</v>
       </c>
       <c r="K167" t="s" s="2">
+        <v>511</v>
+      </c>
+      <c r="L167" t="s" s="2">
         <v>512</v>
-      </c>
-      <c r="L167" t="s" s="2">
-        <v>513</v>
       </c>
       <c r="M167" s="2"/>
       <c r="N167" t="s" s="2">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="O167" t="s" s="2">
         <v>44</v>
@@ -21285,7 +21281,7 @@
         <v>44</v>
       </c>
       <c r="AE167" t="s" s="2">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="AF167" t="s" s="2">
         <v>42</v>
@@ -21309,7 +21305,7 @@
         <v>44</v>
       </c>
       <c r="AM167" t="s" s="2">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AN167" t="s" s="2">
         <v>44</v>
@@ -21317,7 +21313,7 @@
     </row>
     <row r="168">
       <c r="A168" t="s" s="2">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B168" s="2"/>
       <c r="C168" t="s" s="2">
@@ -21343,13 +21339,13 @@
         <v>385</v>
       </c>
       <c r="K168" t="s" s="2">
+        <v>516</v>
+      </c>
+      <c r="L168" t="s" s="2">
         <v>517</v>
       </c>
-      <c r="L168" t="s" s="2">
+      <c r="M168" t="s" s="2">
         <v>518</v>
-      </c>
-      <c r="M168" t="s" s="2">
-        <v>519</v>
       </c>
       <c r="N168" t="s" s="2">
         <v>389</v>
@@ -21401,7 +21397,7 @@
         <v>44</v>
       </c>
       <c r="AE168" t="s" s="2">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="AF168" t="s" s="2">
         <v>42</v>
@@ -21425,7 +21421,7 @@
         <v>44</v>
       </c>
       <c r="AM168" t="s" s="2">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="AN168" t="s" s="2">
         <v>44</v>
@@ -21433,7 +21429,7 @@
     </row>
     <row r="169">
       <c r="A169" t="s" s="2">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B169" s="2"/>
       <c r="C169" t="s" s="2">
@@ -21456,17 +21452,17 @@
         <v>44</v>
       </c>
       <c r="J169" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K169" t="s" s="2">
+        <v>521</v>
+      </c>
+      <c r="L169" t="s" s="2">
         <v>522</v>
-      </c>
-      <c r="L169" t="s" s="2">
-        <v>523</v>
       </c>
       <c r="M169" s="2"/>
       <c r="N169" t="s" s="2">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="O169" t="s" s="2">
         <v>44</v>
@@ -21515,7 +21511,7 @@
         <v>44</v>
       </c>
       <c r="AE169" t="s" s="2">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="AF169" t="s" s="2">
         <v>42</v>
@@ -21530,7 +21526,7 @@
         <v>44</v>
       </c>
       <c r="AJ169" t="s" s="2">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="AK169" t="s" s="2">
         <v>148</v>
@@ -21539,7 +21535,7 @@
         <v>44</v>
       </c>
       <c r="AM169" t="s" s="2">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="AN169" t="s" s="2">
         <v>44</v>
@@ -21547,7 +21543,7 @@
     </row>
     <row r="170">
       <c r="A170" t="s" s="2">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B170" s="2"/>
       <c r="C170" t="s" s="2">
@@ -21576,11 +21572,11 @@
         <v>394</v>
       </c>
       <c r="L170" t="s" s="2">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="M170" s="2"/>
       <c r="N170" t="s" s="2">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="O170" t="s" s="2">
         <v>44</v>
@@ -21629,7 +21625,7 @@
         <v>44</v>
       </c>
       <c r="AE170" t="s" s="2">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="AF170" t="s" s="2">
         <v>42</v>
@@ -21653,7 +21649,7 @@
         <v>44</v>
       </c>
       <c r="AM170" t="s" s="2">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="AN170" t="s" s="2">
         <v>44</v>
@@ -21661,7 +21657,7 @@
     </row>
     <row r="171">
       <c r="A171" t="s" s="2">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B171" s="2"/>
       <c r="C171" t="s" s="2">
@@ -21684,17 +21680,17 @@
         <v>44</v>
       </c>
       <c r="J171" t="s" s="2">
+        <v>530</v>
+      </c>
+      <c r="K171" t="s" s="2">
         <v>531</v>
       </c>
-      <c r="K171" t="s" s="2">
+      <c r="L171" t="s" s="2">
         <v>532</v>
-      </c>
-      <c r="L171" t="s" s="2">
-        <v>533</v>
       </c>
       <c r="M171" s="2"/>
       <c r="N171" t="s" s="2">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="O171" t="s" s="2">
         <v>44</v>
@@ -21743,7 +21739,7 @@
         <v>44</v>
       </c>
       <c r="AE171" t="s" s="2">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AF171" t="s" s="2">
         <v>42</v>
@@ -21752,13 +21748,13 @@
         <v>52</v>
       </c>
       <c r="AH171" t="s" s="2">
+        <v>534</v>
+      </c>
+      <c r="AI171" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ171" t="s" s="2">
         <v>535</v>
-      </c>
-      <c r="AI171" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ171" t="s" s="2">
-        <v>536</v>
       </c>
       <c r="AK171" t="s" s="2">
         <v>148</v>
@@ -21767,7 +21763,7 @@
         <v>44</v>
       </c>
       <c r="AM171" t="s" s="2">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AN171" t="s" s="2">
         <v>44</v>
@@ -21775,7 +21771,7 @@
     </row>
     <row r="172">
       <c r="A172" t="s" s="2">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B172" s="2"/>
       <c r="C172" t="s" s="2">
@@ -21801,10 +21797,10 @@
         <v>241</v>
       </c>
       <c r="K172" t="s" s="2">
+        <v>538</v>
+      </c>
+      <c r="L172" t="s" s="2">
         <v>539</v>
-      </c>
-      <c r="L172" t="s" s="2">
-        <v>540</v>
       </c>
       <c r="M172" s="2"/>
       <c r="N172" s="2"/>
@@ -21855,7 +21851,7 @@
         <v>44</v>
       </c>
       <c r="AE172" t="s" s="2">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AF172" t="s" s="2">
         <v>42</v>
@@ -21870,7 +21866,7 @@
         <v>44</v>
       </c>
       <c r="AJ172" t="s" s="2">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="AK172" t="s" s="2">
         <v>148</v>
@@ -21887,7 +21883,7 @@
     </row>
     <row r="173" hidden="true">
       <c r="A173" t="s" s="2">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B173" s="2"/>
       <c r="C173" t="s" s="2">
@@ -21910,19 +21906,19 @@
         <v>53</v>
       </c>
       <c r="J173" t="s" s="2">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K173" t="s" s="2">
+        <v>542</v>
+      </c>
+      <c r="L173" t="s" s="2">
         <v>543</v>
       </c>
-      <c r="L173" t="s" s="2">
+      <c r="M173" t="s" s="2">
         <v>544</v>
       </c>
-      <c r="M173" t="s" s="2">
+      <c r="N173" t="s" s="2">
         <v>545</v>
-      </c>
-      <c r="N173" t="s" s="2">
-        <v>546</v>
       </c>
       <c r="O173" t="s" s="2">
         <v>44</v>
@@ -21971,7 +21967,7 @@
         <v>44</v>
       </c>
       <c r="AE173" t="s" s="2">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AF173" t="s" s="2">
         <v>42</v>
@@ -21983,10 +21979,10 @@
         <v>44</v>
       </c>
       <c r="AI173" t="s" s="2">
+        <v>546</v>
+      </c>
+      <c r="AJ173" t="s" s="2">
         <v>547</v>
-      </c>
-      <c r="AJ173" t="s" s="2">
-        <v>548</v>
       </c>
       <c r="AK173" t="s" s="2">
         <v>148</v>
@@ -22003,7 +21999,7 @@
     </row>
     <row r="174" hidden="true">
       <c r="A174" t="s" s="2">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B174" s="2"/>
       <c r="C174" t="s" s="2">
@@ -22115,7 +22111,7 @@
     </row>
     <row r="175" hidden="true">
       <c r="A175" t="s" s="2">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B175" s="2"/>
       <c r="C175" t="s" s="2">
@@ -22229,11 +22225,11 @@
     </row>
     <row r="176" hidden="true">
       <c r="A176" t="s" s="2">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B176" s="2"/>
       <c r="C176" t="s" s="2">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D176" s="2"/>
       <c r="E176" t="s" s="2">
@@ -22258,7 +22254,7 @@
         <v>125</v>
       </c>
       <c r="L176" t="s" s="2">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="M176" t="s" s="2">
         <v>127</v>
@@ -22311,7 +22307,7 @@
         <v>44</v>
       </c>
       <c r="AE176" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="AF176" t="s" s="2">
         <v>42</v>
@@ -22343,7 +22339,7 @@
     </row>
     <row r="177" hidden="true">
       <c r="A177" t="s" s="2">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B177" s="2"/>
       <c r="C177" t="s" s="2">
@@ -22369,16 +22365,16 @@
         <v>193</v>
       </c>
       <c r="K177" t="s" s="2">
+        <v>552</v>
+      </c>
+      <c r="L177" t="s" s="2">
         <v>553</v>
       </c>
-      <c r="L177" t="s" s="2">
+      <c r="M177" t="s" s="2">
         <v>554</v>
       </c>
-      <c r="M177" t="s" s="2">
+      <c r="N177" t="s" s="2">
         <v>555</v>
-      </c>
-      <c r="N177" t="s" s="2">
-        <v>556</v>
       </c>
       <c r="O177" t="s" s="2">
         <v>44</v>
@@ -22403,14 +22399,14 @@
         <v>44</v>
       </c>
       <c r="W177" t="s" s="2">
+        <v>556</v>
+      </c>
+      <c r="X177" t="s" s="2">
         <v>557</v>
       </c>
-      <c r="X177" t="s" s="2">
+      <c r="Y177" t="s" s="2">
         <v>558</v>
       </c>
-      <c r="Y177" t="s" s="2">
-        <v>559</v>
-      </c>
       <c r="Z177" t="s" s="2">
         <v>44</v>
       </c>
@@ -22427,7 +22423,7 @@
         <v>44</v>
       </c>
       <c r="AE177" t="s" s="2">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="AF177" t="s" s="2">
         <v>52</v>
@@ -22442,7 +22438,7 @@
         <v>44</v>
       </c>
       <c r="AJ177" t="s" s="2">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AK177" t="s" s="2">
         <v>148</v>
@@ -22451,7 +22447,7 @@
         <v>44</v>
       </c>
       <c r="AM177" t="s" s="2">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="AN177" t="s" s="2">
         <v>44</v>
@@ -22459,7 +22455,7 @@
     </row>
     <row r="178" hidden="true">
       <c r="A178" t="s" s="2">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B178" s="2"/>
       <c r="C178" t="s" s="2">
@@ -22485,16 +22481,16 @@
         <v>193</v>
       </c>
       <c r="K178" t="s" s="2">
+        <v>561</v>
+      </c>
+      <c r="L178" t="s" s="2">
         <v>562</v>
       </c>
-      <c r="L178" t="s" s="2">
+      <c r="M178" t="s" s="2">
         <v>563</v>
       </c>
-      <c r="M178" t="s" s="2">
+      <c r="N178" t="s" s="2">
         <v>564</v>
-      </c>
-      <c r="N178" t="s" s="2">
-        <v>565</v>
       </c>
       <c r="O178" t="s" s="2">
         <v>44</v>
@@ -22519,46 +22515,46 @@
         <v>44</v>
       </c>
       <c r="W178" t="s" s="2">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="X178" t="s" s="2">
+        <v>565</v>
+      </c>
+      <c r="Y178" t="s" s="2">
         <v>566</v>
       </c>
-      <c r="Y178" t="s" s="2">
+      <c r="Z178" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA178" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB178" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC178" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD178" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE178" t="s" s="2">
+        <v>560</v>
+      </c>
+      <c r="AF178" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG178" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH178" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI178" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ178" t="s" s="2">
         <v>567</v>
-      </c>
-      <c r="Z178" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA178" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB178" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC178" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD178" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE178" t="s" s="2">
-        <v>561</v>
-      </c>
-      <c r="AF178" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG178" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH178" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI178" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ178" t="s" s="2">
-        <v>568</v>
       </c>
       <c r="AK178" t="s" s="2">
         <v>148</v>
@@ -22567,7 +22563,7 @@
         <v>44</v>
       </c>
       <c r="AM178" t="s" s="2">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="AN178" t="s" s="2">
         <v>44</v>
@@ -22575,7 +22571,7 @@
     </row>
     <row r="179" hidden="true">
       <c r="A179" t="s" s="2">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B179" s="2"/>
       <c r="C179" t="s" s="2">
@@ -22601,14 +22597,14 @@
         <v>193</v>
       </c>
       <c r="K179" t="s" s="2">
+        <v>570</v>
+      </c>
+      <c r="L179" t="s" s="2">
         <v>571</v>
-      </c>
-      <c r="L179" t="s" s="2">
-        <v>572</v>
       </c>
       <c r="M179" s="2"/>
       <c r="N179" t="s" s="2">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="O179" t="s" s="2">
         <v>44</v>
@@ -22633,46 +22629,46 @@
         <v>44</v>
       </c>
       <c r="W179" t="s" s="2">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="X179" t="s" s="2">
+        <v>573</v>
+      </c>
+      <c r="Y179" t="s" s="2">
         <v>574</v>
       </c>
-      <c r="Y179" t="s" s="2">
+      <c r="Z179" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA179" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB179" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC179" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD179" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE179" t="s" s="2">
+        <v>569</v>
+      </c>
+      <c r="AF179" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG179" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH179" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI179" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ179" t="s" s="2">
         <v>575</v>
-      </c>
-      <c r="Z179" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA179" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB179" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC179" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD179" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE179" t="s" s="2">
-        <v>570</v>
-      </c>
-      <c r="AF179" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG179" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH179" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI179" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ179" t="s" s="2">
-        <v>576</v>
       </c>
       <c r="AK179" t="s" s="2">
         <v>148</v>
@@ -22689,7 +22685,7 @@
     </row>
     <row r="180">
       <c r="A180" t="s" s="2">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B180" s="2"/>
       <c r="C180" t="s" s="2">
@@ -22712,19 +22708,19 @@
         <v>44</v>
       </c>
       <c r="J180" t="s" s="2">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K180" t="s" s="2">
+        <v>577</v>
+      </c>
+      <c r="L180" t="s" s="2">
         <v>578</v>
       </c>
-      <c r="L180" t="s" s="2">
+      <c r="M180" t="s" s="2">
         <v>579</v>
       </c>
-      <c r="M180" t="s" s="2">
+      <c r="N180" t="s" s="2">
         <v>580</v>
-      </c>
-      <c r="N180" t="s" s="2">
-        <v>581</v>
       </c>
       <c r="O180" t="s" s="2">
         <v>44</v>
@@ -22773,7 +22769,7 @@
         <v>44</v>
       </c>
       <c r="AE180" t="s" s="2">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="AF180" t="s" s="2">
         <v>42</v>
@@ -22785,13 +22781,13 @@
         <v>44</v>
       </c>
       <c r="AI180" t="s" s="2">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AJ180" t="s" s="2">
+        <v>581</v>
+      </c>
+      <c r="AK180" t="s" s="2">
         <v>582</v>
-      </c>
-      <c r="AK180" t="s" s="2">
-        <v>583</v>
       </c>
       <c r="AL180" t="s" s="2">
         <v>44</v>
@@ -22805,7 +22801,7 @@
     </row>
     <row r="181" hidden="true">
       <c r="A181" t="s" s="2">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B181" s="2"/>
       <c r="C181" t="s" s="2">
@@ -22917,7 +22913,7 @@
     </row>
     <row r="182" hidden="true">
       <c r="A182" t="s" s="2">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B182" s="2"/>
       <c r="C182" t="s" s="2">
@@ -23031,11 +23027,11 @@
     </row>
     <row r="183" hidden="true">
       <c r="A183" t="s" s="2">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B183" s="2"/>
       <c r="C183" t="s" s="2">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D183" s="2"/>
       <c r="E183" t="s" s="2">
@@ -23060,7 +23056,7 @@
         <v>125</v>
       </c>
       <c r="L183" t="s" s="2">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="M183" t="s" s="2">
         <v>127</v>
@@ -23113,7 +23109,7 @@
         <v>44</v>
       </c>
       <c r="AE183" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="AF183" t="s" s="2">
         <v>42</v>
@@ -23145,7 +23141,7 @@
     </row>
     <row r="184">
       <c r="A184" t="s" s="2">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B184" s="2"/>
       <c r="C184" t="s" s="2">
@@ -23171,16 +23167,16 @@
         <v>193</v>
       </c>
       <c r="K184" t="s" s="2">
+        <v>587</v>
+      </c>
+      <c r="L184" t="s" s="2">
         <v>588</v>
       </c>
-      <c r="L184" t="s" s="2">
+      <c r="M184" t="s" s="2">
         <v>589</v>
       </c>
-      <c r="M184" t="s" s="2">
+      <c r="N184" t="s" s="2">
         <v>590</v>
-      </c>
-      <c r="N184" t="s" s="2">
-        <v>591</v>
       </c>
       <c r="O184" t="s" s="2">
         <v>44</v>
@@ -23209,49 +23205,49 @@
       </c>
       <c r="X184" s="2"/>
       <c r="Y184" t="s" s="2">
+        <v>591</v>
+      </c>
+      <c r="Z184" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA184" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB184" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC184" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD184" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE184" t="s" s="2">
+        <v>586</v>
+      </c>
+      <c r="AF184" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AG184" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH184" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI184" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ184" t="s" s="2">
         <v>592</v>
       </c>
-      <c r="Z184" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA184" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB184" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC184" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD184" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE184" t="s" s="2">
-        <v>587</v>
-      </c>
-      <c r="AF184" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AG184" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH184" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI184" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ184" t="s" s="2">
+      <c r="AK184" t="s" s="2">
         <v>593</v>
       </c>
-      <c r="AK184" t="s" s="2">
+      <c r="AL184" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM184" t="s" s="2">
         <v>594</v>
-      </c>
-      <c r="AL184" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM184" t="s" s="2">
-        <v>595</v>
       </c>
       <c r="AN184" t="s" s="2">
         <v>44</v>
@@ -23259,7 +23255,7 @@
     </row>
     <row r="185">
       <c r="A185" t="s" s="2">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B185" s="2"/>
       <c r="C185" t="s" s="2">
@@ -23285,16 +23281,16 @@
         <v>367</v>
       </c>
       <c r="K185" t="s" s="2">
+        <v>596</v>
+      </c>
+      <c r="L185" t="s" s="2">
         <v>597</v>
       </c>
-      <c r="L185" t="s" s="2">
+      <c r="M185" t="s" s="2">
         <v>598</v>
       </c>
-      <c r="M185" t="s" s="2">
+      <c r="N185" t="s" s="2">
         <v>599</v>
-      </c>
-      <c r="N185" t="s" s="2">
-        <v>600</v>
       </c>
       <c r="O185" t="s" s="2">
         <v>44</v>
@@ -23343,7 +23339,7 @@
         <v>44</v>
       </c>
       <c r="AE185" t="s" s="2">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="AF185" t="s" s="2">
         <v>42</v>
@@ -23358,16 +23354,16 @@
         <v>44</v>
       </c>
       <c r="AJ185" t="s" s="2">
+        <v>600</v>
+      </c>
+      <c r="AK185" t="s" s="2">
         <v>601</v>
       </c>
-      <c r="AK185" t="s" s="2">
+      <c r="AL185" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM185" t="s" s="2">
         <v>602</v>
-      </c>
-      <c r="AL185" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM185" t="s" s="2">
-        <v>603</v>
       </c>
       <c r="AN185" t="s" s="2">
         <v>44</v>
@@ -23375,14 +23371,14 @@
     </row>
     <row r="186">
       <c r="A186" t="s" s="2">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B186" s="2"/>
       <c r="C186" t="s" s="2">
+        <v>604</v>
+      </c>
+      <c r="D186" t="s" s="2">
         <v>605</v>
-      </c>
-      <c r="D186" t="s" s="2">
-        <v>606</v>
       </c>
       <c r="E186" t="s" s="2">
         <v>42</v>
@@ -23400,16 +23396,16 @@
         <v>44</v>
       </c>
       <c r="J186" t="s" s="2">
+        <v>606</v>
+      </c>
+      <c r="K186" t="s" s="2">
         <v>607</v>
       </c>
-      <c r="K186" t="s" s="2">
+      <c r="L186" t="s" s="2">
         <v>608</v>
       </c>
-      <c r="L186" t="s" s="2">
+      <c r="M186" t="s" s="2">
         <v>609</v>
-      </c>
-      <c r="M186" t="s" s="2">
-        <v>610</v>
       </c>
       <c r="N186" s="2"/>
       <c r="O186" t="s" s="2">
@@ -23459,7 +23455,7 @@
         <v>44</v>
       </c>
       <c r="AE186" t="s" s="2">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AF186" t="s" s="2">
         <v>42</v>
@@ -23474,7 +23470,7 @@
         <v>44</v>
       </c>
       <c r="AJ186" t="s" s="2">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="AK186" t="s" s="2">
         <v>148</v>
@@ -23483,7 +23479,7 @@
         <v>44</v>
       </c>
       <c r="AM186" t="s" s="2">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="AN186" t="s" s="2">
         <v>44</v>
@@ -23491,14 +23487,14 @@
     </row>
     <row r="187">
       <c r="A187" t="s" s="2">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B187" s="2"/>
       <c r="C187" t="s" s="2">
         <v>44</v>
       </c>
       <c r="D187" t="s" s="2">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E187" t="s" s="2">
         <v>42</v>
@@ -23516,19 +23512,19 @@
         <v>53</v>
       </c>
       <c r="J187" t="s" s="2">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="K187" t="s" s="2">
+        <v>614</v>
+      </c>
+      <c r="L187" t="s" s="2">
         <v>615</v>
       </c>
-      <c r="L187" t="s" s="2">
+      <c r="M187" t="s" s="2">
         <v>616</v>
       </c>
-      <c r="M187" t="s" s="2">
+      <c r="N187" t="s" s="2">
         <v>617</v>
-      </c>
-      <c r="N187" t="s" s="2">
-        <v>618</v>
       </c>
       <c r="O187" t="s" s="2">
         <v>44</v>
@@ -23577,7 +23573,7 @@
         <v>44</v>
       </c>
       <c r="AE187" t="s" s="2">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AF187" t="s" s="2">
         <v>42</v>
@@ -23592,10 +23588,10 @@
         <v>44</v>
       </c>
       <c r="AJ187" t="s" s="2">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="AK187" t="s" s="2">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="AL187" t="s" s="2">
         <v>44</v>
@@ -23609,7 +23605,7 @@
     </row>
     <row r="188" hidden="true">
       <c r="A188" t="s" s="2">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B188" s="2"/>
       <c r="C188" t="s" s="2">
@@ -23632,19 +23628,19 @@
         <v>53</v>
       </c>
       <c r="J188" t="s" s="2">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K188" t="s" s="2">
+        <v>620</v>
+      </c>
+      <c r="L188" t="s" s="2">
         <v>621</v>
       </c>
-      <c r="L188" t="s" s="2">
+      <c r="M188" t="s" s="2">
         <v>622</v>
       </c>
-      <c r="M188" t="s" s="2">
+      <c r="N188" t="s" s="2">
         <v>623</v>
-      </c>
-      <c r="N188" t="s" s="2">
-        <v>624</v>
       </c>
       <c r="O188" t="s" s="2">
         <v>44</v>
@@ -23693,7 +23689,7 @@
         <v>44</v>
       </c>
       <c r="AE188" t="s" s="2">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="AF188" t="s" s="2">
         <v>42</v>
@@ -23705,10 +23701,10 @@
         <v>44</v>
       </c>
       <c r="AI188" t="s" s="2">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AJ188" t="s" s="2">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="AK188" t="s" s="2">
         <v>148</v>
@@ -23725,7 +23721,7 @@
     </row>
     <row r="189" hidden="true">
       <c r="A189" t="s" s="2">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B189" s="2"/>
       <c r="C189" t="s" s="2">
@@ -23837,7 +23833,7 @@
     </row>
     <row r="190" hidden="true">
       <c r="A190" t="s" s="2">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B190" s="2"/>
       <c r="C190" t="s" s="2">
@@ -23951,11 +23947,11 @@
     </row>
     <row r="191" hidden="true">
       <c r="A191" t="s" s="2">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B191" s="2"/>
       <c r="C191" t="s" s="2">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D191" s="2"/>
       <c r="E191" t="s" s="2">
@@ -23980,7 +23976,7 @@
         <v>125</v>
       </c>
       <c r="L191" t="s" s="2">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="M191" t="s" s="2">
         <v>127</v>
@@ -24033,7 +24029,7 @@
         <v>44</v>
       </c>
       <c r="AE191" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="AF191" t="s" s="2">
         <v>42</v>
@@ -24065,7 +24061,7 @@
     </row>
     <row r="192" hidden="true">
       <c r="A192" t="s" s="2">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B192" s="2"/>
       <c r="C192" t="s" s="2">
@@ -24088,16 +24084,16 @@
         <v>53</v>
       </c>
       <c r="J192" t="s" s="2">
+        <v>629</v>
+      </c>
+      <c r="K192" t="s" s="2">
         <v>630</v>
       </c>
-      <c r="K192" t="s" s="2">
+      <c r="L192" t="s" s="2">
         <v>631</v>
       </c>
-      <c r="L192" t="s" s="2">
+      <c r="M192" t="s" s="2">
         <v>632</v>
-      </c>
-      <c r="M192" t="s" s="2">
-        <v>633</v>
       </c>
       <c r="N192" s="2"/>
       <c r="O192" t="s" s="2">
@@ -24147,7 +24143,7 @@
         <v>44</v>
       </c>
       <c r="AE192" t="s" s="2">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AF192" t="s" s="2">
         <v>52</v>
@@ -24171,7 +24167,7 @@
         <v>44</v>
       </c>
       <c r="AM192" t="s" s="2">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="AN192" t="s" s="2">
         <v>44</v>
@@ -24179,7 +24175,7 @@
     </row>
     <row r="193" hidden="true">
       <c r="A193" t="s" s="2">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B193" s="2"/>
       <c r="C193" t="s" s="2">
@@ -24205,10 +24201,10 @@
         <v>71</v>
       </c>
       <c r="K193" t="s" s="2">
+        <v>635</v>
+      </c>
+      <c r="L193" t="s" s="2">
         <v>636</v>
-      </c>
-      <c r="L193" t="s" s="2">
-        <v>637</v>
       </c>
       <c r="M193" s="2"/>
       <c r="N193" s="2"/>
@@ -24238,43 +24234,43 @@
         <v>170</v>
       </c>
       <c r="X193" t="s" s="2">
+        <v>636</v>
+      </c>
+      <c r="Y193" t="s" s="2">
         <v>637</v>
       </c>
-      <c r="Y193" t="s" s="2">
+      <c r="Z193" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA193" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB193" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC193" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD193" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE193" t="s" s="2">
+        <v>634</v>
+      </c>
+      <c r="AF193" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AG193" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH193" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI193" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ193" t="s" s="2">
         <v>638</v>
-      </c>
-      <c r="Z193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE193" t="s" s="2">
-        <v>635</v>
-      </c>
-      <c r="AF193" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AG193" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ193" t="s" s="2">
-        <v>639</v>
       </c>
       <c r="AK193" t="s" s="2">
         <v>148</v>

</xml_diff>

<commit_message>
Regenerated after merging SML into master (relates to #26) with updated aubase location and changes to patient and pracitioner profiles to remove must support from prohibited elements (related to #40) and Base Medication profile (Fixes #41)
</commit_message>
<xml_diff>
--- a/output/AdvanceCareRecords/patient-dh-base-1.xlsx
+++ b/output/AdvanceCareRecords/patient-dh-base-1.xlsx
@@ -20515,7 +20515,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" hidden="true">
       <c r="A161" t="s" s="2">
         <v>482</v>
       </c>
@@ -20531,7 +20531,7 @@
         <v>42</v>
       </c>
       <c r="G161" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H161" t="s" s="2">
         <v>44</v>

</xml_diff>

<commit_message>
Advance Care Records, Event Summary, Personal Health Records, Shared Health Summary and Shared Medicines List Implementation Guides (IGs) have been regenerated after a range of profile and examples updates. Updated IGs reflect the feature updates completed till date.
</commit_message>
<xml_diff>
--- a/output/AdvanceCareRecords/patient-dh-base-1.xlsx
+++ b/output/AdvanceCareRecords/patient-dh-base-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7395" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7395" uniqueCount="648">
   <si>
     <t>Path</t>
   </si>
@@ -1439,10 +1439,6 @@
   </si>
   <si>
     <t>Patient.birthDate.value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-</t>
   </si>
   <si>
     <t>Primitive value for date</t>
@@ -20658,13 +20654,13 @@
         <v>44</v>
       </c>
       <c r="J162" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="K162" t="s" s="2">
         <v>447</v>
       </c>
-      <c r="K162" t="s" s="2">
+      <c r="L162" t="s" s="2">
         <v>448</v>
-      </c>
-      <c r="L162" t="s" s="2">
-        <v>449</v>
       </c>
       <c r="M162" s="2"/>
       <c r="N162" s="2"/>
@@ -20715,7 +20711,7 @@
         <v>44</v>
       </c>
       <c r="AE162" t="s" s="2">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AF162" t="s" s="2">
         <v>42</v>
@@ -20747,7 +20743,7 @@
     </row>
     <row r="163" hidden="true">
       <c r="A163" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" t="s" s="2">
@@ -20770,19 +20766,19 @@
         <v>53</v>
       </c>
       <c r="J163" t="s" s="2">
+        <v>451</v>
+      </c>
+      <c r="K163" t="s" s="2">
         <v>452</v>
       </c>
-      <c r="K163" t="s" s="2">
+      <c r="L163" t="s" s="2">
         <v>453</v>
       </c>
-      <c r="L163" t="s" s="2">
+      <c r="M163" t="s" s="2">
         <v>454</v>
       </c>
-      <c r="M163" t="s" s="2">
+      <c r="N163" t="s" s="2">
         <v>455</v>
-      </c>
-      <c r="N163" t="s" s="2">
-        <v>456</v>
       </c>
       <c r="O163" t="s" s="2">
         <v>44</v>
@@ -20829,7 +20825,7 @@
         <v>182</v>
       </c>
       <c r="AE163" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="AF163" t="s" s="2">
         <v>42</v>
@@ -20844,7 +20840,7 @@
         <v>44</v>
       </c>
       <c r="AJ163" t="s" s="2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AK163" t="s" s="2">
         <v>114</v>
@@ -20853,7 +20849,7 @@
         <v>44</v>
       </c>
       <c r="AM163" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="AN163" t="s" s="2">
         <v>44</v>
@@ -20861,10 +20857,10 @@
     </row>
     <row r="164">
       <c r="A164" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B164" t="s" s="2">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C164" t="s" s="2">
         <v>44</v>
@@ -20889,16 +20885,16 @@
         <v>381</v>
       </c>
       <c r="K164" t="s" s="2">
+        <v>459</v>
+      </c>
+      <c r="L164" t="s" s="2">
         <v>460</v>
       </c>
-      <c r="L164" t="s" s="2">
-        <v>461</v>
-      </c>
       <c r="M164" t="s" s="2">
+        <v>454</v>
+      </c>
+      <c r="N164" t="s" s="2">
         <v>455</v>
-      </c>
-      <c r="N164" t="s" s="2">
-        <v>456</v>
       </c>
       <c r="O164" t="s" s="2">
         <v>44</v>
@@ -20947,7 +20943,7 @@
         <v>44</v>
       </c>
       <c r="AE164" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="AF164" t="s" s="2">
         <v>42</v>
@@ -20962,7 +20958,7 @@
         <v>44</v>
       </c>
       <c r="AJ164" t="s" s="2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AK164" t="s" s="2">
         <v>114</v>
@@ -20971,7 +20967,7 @@
         <v>44</v>
       </c>
       <c r="AM164" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="AN164" t="s" s="2">
         <v>44</v>
@@ -20979,10 +20975,10 @@
     </row>
     <row r="165">
       <c r="A165" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B165" t="s" s="2">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C165" t="s" s="2">
         <v>44</v>
@@ -21007,16 +21003,16 @@
         <v>286</v>
       </c>
       <c r="K165" t="s" s="2">
+        <v>462</v>
+      </c>
+      <c r="L165" t="s" s="2">
         <v>463</v>
       </c>
-      <c r="L165" t="s" s="2">
-        <v>464</v>
-      </c>
       <c r="M165" t="s" s="2">
+        <v>454</v>
+      </c>
+      <c r="N165" t="s" s="2">
         <v>455</v>
-      </c>
-      <c r="N165" t="s" s="2">
-        <v>456</v>
       </c>
       <c r="O165" t="s" s="2">
         <v>44</v>
@@ -21065,7 +21061,7 @@
         <v>44</v>
       </c>
       <c r="AE165" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="AF165" t="s" s="2">
         <v>42</v>
@@ -21080,7 +21076,7 @@
         <v>44</v>
       </c>
       <c r="AJ165" t="s" s="2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AK165" t="s" s="2">
         <v>114</v>
@@ -21089,7 +21085,7 @@
         <v>44</v>
       </c>
       <c r="AM165" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="AN165" t="s" s="2">
         <v>44</v>
@@ -21097,7 +21093,7 @@
     </row>
     <row r="166" hidden="true">
       <c r="A166" t="s" s="2">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B166" s="2"/>
       <c r="C166" t="s" s="2">
@@ -21209,7 +21205,7 @@
     </row>
     <row r="167" hidden="true">
       <c r="A167" t="s" s="2">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B167" s="2"/>
       <c r="C167" t="s" s="2">
@@ -21319,7 +21315,7 @@
     </row>
     <row r="168">
       <c r="A168" t="s" s="2">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B168" t="s" s="2">
         <v>431</v>
@@ -21435,7 +21431,7 @@
     </row>
     <row r="169" hidden="true">
       <c r="A169" t="s" s="2">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B169" s="2"/>
       <c r="C169" t="s" s="2">
@@ -21458,13 +21454,13 @@
         <v>44</v>
       </c>
       <c r="J169" t="s" s="2">
-        <v>447</v>
+        <v>286</v>
       </c>
       <c r="K169" t="s" s="2">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="L169" t="s" s="2">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="M169" s="2"/>
       <c r="N169" s="2"/>
@@ -21515,7 +21511,7 @@
         <v>44</v>
       </c>
       <c r="AE169" t="s" s="2">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="AF169" t="s" s="2">
         <v>42</v>
@@ -21547,7 +21543,7 @@
     </row>
     <row r="170">
       <c r="A170" t="s" s="2">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B170" s="2"/>
       <c r="C170" t="s" s="2">
@@ -21573,16 +21569,16 @@
         <v>130</v>
       </c>
       <c r="K170" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="L170" t="s" s="2">
         <v>471</v>
       </c>
-      <c r="L170" t="s" s="2">
+      <c r="M170" t="s" s="2">
         <v>472</v>
       </c>
-      <c r="M170" t="s" s="2">
+      <c r="N170" t="s" s="2">
         <v>473</v>
-      </c>
-      <c r="N170" t="s" s="2">
-        <v>474</v>
       </c>
       <c r="O170" t="s" s="2">
         <v>44</v>
@@ -21631,7 +21627,7 @@
         <v>44</v>
       </c>
       <c r="AE170" t="s" s="2">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="AF170" t="s" s="2">
         <v>42</v>
@@ -21646,16 +21642,16 @@
         <v>44</v>
       </c>
       <c r="AJ170" t="s" s="2">
+        <v>474</v>
+      </c>
+      <c r="AK170" t="s" s="2">
         <v>475</v>
       </c>
-      <c r="AK170" t="s" s="2">
+      <c r="AL170" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM170" t="s" s="2">
         <v>476</v>
-      </c>
-      <c r="AL170" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM170" t="s" s="2">
-        <v>477</v>
       </c>
       <c r="AN170" t="s" s="2">
         <v>44</v>
@@ -21663,7 +21659,7 @@
     </row>
     <row r="171">
       <c r="A171" t="s" s="2">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B171" s="2"/>
       <c r="C171" t="s" s="2">
@@ -21689,14 +21685,14 @@
         <v>207</v>
       </c>
       <c r="K171" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="L171" t="s" s="2">
         <v>479</v>
-      </c>
-      <c r="L171" t="s" s="2">
-        <v>480</v>
       </c>
       <c r="M171" s="2"/>
       <c r="N171" t="s" s="2">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="O171" t="s" s="2">
         <v>44</v>
@@ -21724,52 +21720,52 @@
         <v>75</v>
       </c>
       <c r="X171" t="s" s="2">
+        <v>481</v>
+      </c>
+      <c r="Y171" t="s" s="2">
         <v>482</v>
       </c>
-      <c r="Y171" t="s" s="2">
+      <c r="Z171" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA171" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB171" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC171" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD171" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE171" t="s" s="2">
+        <v>477</v>
+      </c>
+      <c r="AF171" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG171" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH171" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI171" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ171" t="s" s="2">
         <v>483</v>
       </c>
-      <c r="Z171" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA171" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB171" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC171" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD171" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE171" t="s" s="2">
-        <v>478</v>
-      </c>
-      <c r="AF171" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG171" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH171" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI171" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ171" t="s" s="2">
+      <c r="AK171" t="s" s="2">
         <v>484</v>
       </c>
-      <c r="AK171" t="s" s="2">
+      <c r="AL171" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM171" t="s" s="2">
         <v>485</v>
-      </c>
-      <c r="AL171" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM171" t="s" s="2">
-        <v>486</v>
       </c>
       <c r="AN171" t="s" s="2">
         <v>44</v>
@@ -21777,7 +21773,7 @@
     </row>
     <row r="172">
       <c r="A172" t="s" s="2">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B172" s="2"/>
       <c r="C172" t="s" s="2">
@@ -21800,19 +21796,19 @@
         <v>44</v>
       </c>
       <c r="J172" t="s" s="2">
+        <v>487</v>
+      </c>
+      <c r="K172" t="s" s="2">
         <v>488</v>
       </c>
-      <c r="K172" t="s" s="2">
+      <c r="L172" t="s" s="2">
         <v>489</v>
       </c>
-      <c r="L172" t="s" s="2">
+      <c r="M172" t="s" s="2">
         <v>490</v>
       </c>
-      <c r="M172" t="s" s="2">
+      <c r="N172" t="s" s="2">
         <v>491</v>
-      </c>
-      <c r="N172" t="s" s="2">
-        <v>492</v>
       </c>
       <c r="O172" t="s" s="2">
         <v>44</v>
@@ -21861,7 +21857,7 @@
         <v>44</v>
       </c>
       <c r="AE172" t="s" s="2">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="AF172" t="s" s="2">
         <v>42</v>
@@ -21876,7 +21872,7 @@
         <v>44</v>
       </c>
       <c r="AJ172" t="s" s="2">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="AK172" t="s" s="2">
         <v>114</v>
@@ -21885,7 +21881,7 @@
         <v>44</v>
       </c>
       <c r="AM172" t="s" s="2">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="AN172" t="s" s="2">
         <v>44</v>
@@ -21893,7 +21889,7 @@
     </row>
     <row r="173" hidden="true">
       <c r="A173" t="s" s="2">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B173" s="2"/>
       <c r="C173" t="s" s="2">
@@ -21916,17 +21912,17 @@
         <v>44</v>
       </c>
       <c r="J173" t="s" s="2">
+        <v>495</v>
+      </c>
+      <c r="K173" t="s" s="2">
         <v>496</v>
       </c>
-      <c r="K173" t="s" s="2">
+      <c r="L173" t="s" s="2">
         <v>497</v>
-      </c>
-      <c r="L173" t="s" s="2">
-        <v>498</v>
       </c>
       <c r="M173" s="2"/>
       <c r="N173" t="s" s="2">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="O173" t="s" s="2">
         <v>44</v>
@@ -21975,7 +21971,7 @@
         <v>44</v>
       </c>
       <c r="AE173" t="s" s="2">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="AF173" t="s" s="2">
         <v>42</v>
@@ -21990,7 +21986,7 @@
         <v>44</v>
       </c>
       <c r="AJ173" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AK173" t="s" s="2">
         <v>114</v>
@@ -21999,7 +21995,7 @@
         <v>44</v>
       </c>
       <c r="AM173" t="s" s="2">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="AN173" t="s" s="2">
         <v>44</v>
@@ -22007,7 +22003,7 @@
     </row>
     <row r="174">
       <c r="A174" t="s" s="2">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B174" s="2"/>
       <c r="C174" t="s" s="2">
@@ -22030,19 +22026,19 @@
         <v>44</v>
       </c>
       <c r="J174" t="s" s="2">
+        <v>502</v>
+      </c>
+      <c r="K174" t="s" s="2">
         <v>503</v>
       </c>
-      <c r="K174" t="s" s="2">
+      <c r="L174" t="s" s="2">
         <v>504</v>
       </c>
-      <c r="L174" t="s" s="2">
+      <c r="M174" t="s" s="2">
         <v>505</v>
       </c>
-      <c r="M174" t="s" s="2">
+      <c r="N174" t="s" s="2">
         <v>506</v>
-      </c>
-      <c r="N174" t="s" s="2">
-        <v>507</v>
       </c>
       <c r="O174" t="s" s="2">
         <v>44</v>
@@ -22091,7 +22087,7 @@
         <v>44</v>
       </c>
       <c r="AE174" t="s" s="2">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AF174" t="s" s="2">
         <v>42</v>
@@ -22103,10 +22099,10 @@
         <v>44</v>
       </c>
       <c r="AI174" t="s" s="2">
+        <v>507</v>
+      </c>
+      <c r="AJ174" t="s" s="2">
         <v>508</v>
-      </c>
-      <c r="AJ174" t="s" s="2">
-        <v>509</v>
       </c>
       <c r="AK174" t="s" s="2">
         <v>114</v>
@@ -22123,7 +22119,7 @@
     </row>
     <row r="175" hidden="true">
       <c r="A175" t="s" s="2">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B175" s="2"/>
       <c r="C175" t="s" s="2">
@@ -22235,7 +22231,7 @@
     </row>
     <row r="176" hidden="true">
       <c r="A176" t="s" s="2">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B176" s="2"/>
       <c r="C176" t="s" s="2">
@@ -22349,11 +22345,11 @@
     </row>
     <row r="177" hidden="true">
       <c r="A177" t="s" s="2">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B177" s="2"/>
       <c r="C177" t="s" s="2">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D177" s="2"/>
       <c r="E177" t="s" s="2">
@@ -22378,7 +22374,7 @@
         <v>152</v>
       </c>
       <c r="L177" t="s" s="2">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="M177" t="s" s="2">
         <v>119</v>
@@ -22431,7 +22427,7 @@
         <v>44</v>
       </c>
       <c r="AE177" t="s" s="2">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AF177" t="s" s="2">
         <v>42</v>
@@ -22463,7 +22459,7 @@
     </row>
     <row r="178">
       <c r="A178" t="s" s="2">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B178" s="2"/>
       <c r="C178" t="s" s="2">
@@ -22489,14 +22485,14 @@
         <v>207</v>
       </c>
       <c r="K178" t="s" s="2">
+        <v>516</v>
+      </c>
+      <c r="L178" t="s" s="2">
         <v>517</v>
-      </c>
-      <c r="L178" t="s" s="2">
-        <v>518</v>
       </c>
       <c r="M178" s="2"/>
       <c r="N178" t="s" s="2">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="O178" t="s" s="2">
         <v>44</v>
@@ -22525,7 +22521,7 @@
       </c>
       <c r="X178" s="2"/>
       <c r="Y178" t="s" s="2">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="Z178" t="s" s="2">
         <v>44</v>
@@ -22543,7 +22539,7 @@
         <v>44</v>
       </c>
       <c r="AE178" t="s" s="2">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="AF178" t="s" s="2">
         <v>42</v>
@@ -22558,7 +22554,7 @@
         <v>44</v>
       </c>
       <c r="AJ178" t="s" s="2">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="AK178" t="s" s="2">
         <v>114</v>
@@ -22567,7 +22563,7 @@
         <v>44</v>
       </c>
       <c r="AM178" t="s" s="2">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="AN178" t="s" s="2">
         <v>44</v>
@@ -22575,7 +22571,7 @@
     </row>
     <row r="179">
       <c r="A179" t="s" s="2">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B179" s="2"/>
       <c r="C179" t="s" s="2">
@@ -22610,7 +22606,7 @@
         <v>393</v>
       </c>
       <c r="N179" t="s" s="2">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="O179" t="s" s="2">
         <v>44</v>
@@ -22659,7 +22655,7 @@
         <v>44</v>
       </c>
       <c r="AE179" t="s" s="2">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="AF179" t="s" s="2">
         <v>42</v>
@@ -22691,7 +22687,7 @@
     </row>
     <row r="180">
       <c r="A180" t="s" s="2">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B180" s="2"/>
       <c r="C180" t="s" s="2">
@@ -22717,13 +22713,13 @@
         <v>399</v>
       </c>
       <c r="K180" t="s" s="2">
+        <v>525</v>
+      </c>
+      <c r="L180" t="s" s="2">
         <v>526</v>
       </c>
-      <c r="L180" t="s" s="2">
+      <c r="M180" t="s" s="2">
         <v>527</v>
-      </c>
-      <c r="M180" t="s" s="2">
-        <v>528</v>
       </c>
       <c r="N180" t="s" s="2">
         <v>403</v>
@@ -22775,7 +22771,7 @@
         <v>44</v>
       </c>
       <c r="AE180" t="s" s="2">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="AF180" t="s" s="2">
         <v>42</v>
@@ -22799,7 +22795,7 @@
         <v>44</v>
       </c>
       <c r="AM180" t="s" s="2">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="AN180" t="s" s="2">
         <v>44</v>
@@ -22807,7 +22803,7 @@
     </row>
     <row r="181">
       <c r="A181" t="s" s="2">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B181" s="2"/>
       <c r="C181" t="s" s="2">
@@ -22833,14 +22829,14 @@
         <v>130</v>
       </c>
       <c r="K181" t="s" s="2">
+        <v>530</v>
+      </c>
+      <c r="L181" t="s" s="2">
         <v>531</v>
-      </c>
-      <c r="L181" t="s" s="2">
-        <v>532</v>
       </c>
       <c r="M181" s="2"/>
       <c r="N181" t="s" s="2">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="O181" t="s" s="2">
         <v>44</v>
@@ -22889,7 +22885,7 @@
         <v>44</v>
       </c>
       <c r="AE181" t="s" s="2">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AF181" t="s" s="2">
         <v>42</v>
@@ -22904,7 +22900,7 @@
         <v>44</v>
       </c>
       <c r="AJ181" t="s" s="2">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="AK181" t="s" s="2">
         <v>114</v>
@@ -22913,7 +22909,7 @@
         <v>44</v>
       </c>
       <c r="AM181" t="s" s="2">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="AN181" t="s" s="2">
         <v>44</v>
@@ -22921,7 +22917,7 @@
     </row>
     <row r="182">
       <c r="A182" t="s" s="2">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B182" s="2"/>
       <c r="C182" t="s" s="2">
@@ -22950,11 +22946,11 @@
         <v>408</v>
       </c>
       <c r="L182" t="s" s="2">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="M182" s="2"/>
       <c r="N182" t="s" s="2">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="O182" t="s" s="2">
         <v>44</v>
@@ -23003,7 +22999,7 @@
         <v>44</v>
       </c>
       <c r="AE182" t="s" s="2">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="AF182" t="s" s="2">
         <v>42</v>
@@ -23027,7 +23023,7 @@
         <v>44</v>
       </c>
       <c r="AM182" t="s" s="2">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AN182" t="s" s="2">
         <v>44</v>
@@ -23035,7 +23031,7 @@
     </row>
     <row r="183">
       <c r="A183" t="s" s="2">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B183" s="2"/>
       <c r="C183" t="s" s="2">
@@ -23058,17 +23054,17 @@
         <v>44</v>
       </c>
       <c r="J183" t="s" s="2">
+        <v>539</v>
+      </c>
+      <c r="K183" t="s" s="2">
         <v>540</v>
       </c>
-      <c r="K183" t="s" s="2">
+      <c r="L183" t="s" s="2">
         <v>541</v>
-      </c>
-      <c r="L183" t="s" s="2">
-        <v>542</v>
       </c>
       <c r="M183" s="2"/>
       <c r="N183" t="s" s="2">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="O183" t="s" s="2">
         <v>44</v>
@@ -23117,7 +23113,7 @@
         <v>44</v>
       </c>
       <c r="AE183" t="s" s="2">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AF183" t="s" s="2">
         <v>42</v>
@@ -23126,13 +23122,13 @@
         <v>52</v>
       </c>
       <c r="AH183" t="s" s="2">
+        <v>543</v>
+      </c>
+      <c r="AI183" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ183" t="s" s="2">
         <v>544</v>
-      </c>
-      <c r="AI183" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ183" t="s" s="2">
-        <v>545</v>
       </c>
       <c r="AK183" t="s" s="2">
         <v>114</v>
@@ -23141,7 +23137,7 @@
         <v>44</v>
       </c>
       <c r="AM183" t="s" s="2">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="AN183" t="s" s="2">
         <v>44</v>
@@ -23149,7 +23145,7 @@
     </row>
     <row r="184">
       <c r="A184" t="s" s="2">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B184" s="2"/>
       <c r="C184" t="s" s="2">
@@ -23175,10 +23171,10 @@
         <v>255</v>
       </c>
       <c r="K184" t="s" s="2">
+        <v>547</v>
+      </c>
+      <c r="L184" t="s" s="2">
         <v>548</v>
-      </c>
-      <c r="L184" t="s" s="2">
-        <v>549</v>
       </c>
       <c r="M184" s="2"/>
       <c r="N184" s="2"/>
@@ -23229,7 +23225,7 @@
         <v>44</v>
       </c>
       <c r="AE184" t="s" s="2">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AF184" t="s" s="2">
         <v>42</v>
@@ -23244,7 +23240,7 @@
         <v>44</v>
       </c>
       <c r="AJ184" t="s" s="2">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AK184" t="s" s="2">
         <v>114</v>
@@ -23261,7 +23257,7 @@
     </row>
     <row r="185" hidden="true">
       <c r="A185" t="s" s="2">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B185" s="2"/>
       <c r="C185" t="s" s="2">
@@ -23284,19 +23280,19 @@
         <v>53</v>
       </c>
       <c r="J185" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K185" t="s" s="2">
+        <v>551</v>
+      </c>
+      <c r="L185" t="s" s="2">
         <v>552</v>
       </c>
-      <c r="L185" t="s" s="2">
+      <c r="M185" t="s" s="2">
         <v>553</v>
       </c>
-      <c r="M185" t="s" s="2">
+      <c r="N185" t="s" s="2">
         <v>554</v>
-      </c>
-      <c r="N185" t="s" s="2">
-        <v>555</v>
       </c>
       <c r="O185" t="s" s="2">
         <v>44</v>
@@ -23345,7 +23341,7 @@
         <v>44</v>
       </c>
       <c r="AE185" t="s" s="2">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="AF185" t="s" s="2">
         <v>42</v>
@@ -23357,10 +23353,10 @@
         <v>44</v>
       </c>
       <c r="AI185" t="s" s="2">
+        <v>555</v>
+      </c>
+      <c r="AJ185" t="s" s="2">
         <v>556</v>
-      </c>
-      <c r="AJ185" t="s" s="2">
-        <v>557</v>
       </c>
       <c r="AK185" t="s" s="2">
         <v>114</v>
@@ -23377,7 +23373,7 @@
     </row>
     <row r="186" hidden="true">
       <c r="A186" t="s" s="2">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B186" s="2"/>
       <c r="C186" t="s" s="2">
@@ -23489,7 +23485,7 @@
     </row>
     <row r="187" hidden="true">
       <c r="A187" t="s" s="2">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B187" s="2"/>
       <c r="C187" t="s" s="2">
@@ -23603,11 +23599,11 @@
     </row>
     <row r="188" hidden="true">
       <c r="A188" t="s" s="2">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B188" s="2"/>
       <c r="C188" t="s" s="2">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D188" s="2"/>
       <c r="E188" t="s" s="2">
@@ -23632,7 +23628,7 @@
         <v>152</v>
       </c>
       <c r="L188" t="s" s="2">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="M188" t="s" s="2">
         <v>119</v>
@@ -23685,7 +23681,7 @@
         <v>44</v>
       </c>
       <c r="AE188" t="s" s="2">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AF188" t="s" s="2">
         <v>42</v>
@@ -23717,7 +23713,7 @@
     </row>
     <row r="189" hidden="true">
       <c r="A189" t="s" s="2">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B189" s="2"/>
       <c r="C189" t="s" s="2">
@@ -23743,16 +23739,16 @@
         <v>207</v>
       </c>
       <c r="K189" t="s" s="2">
+        <v>561</v>
+      </c>
+      <c r="L189" t="s" s="2">
         <v>562</v>
       </c>
-      <c r="L189" t="s" s="2">
+      <c r="M189" t="s" s="2">
         <v>563</v>
       </c>
-      <c r="M189" t="s" s="2">
+      <c r="N189" t="s" s="2">
         <v>564</v>
-      </c>
-      <c r="N189" t="s" s="2">
-        <v>565</v>
       </c>
       <c r="O189" t="s" s="2">
         <v>44</v>
@@ -23777,14 +23773,14 @@
         <v>44</v>
       </c>
       <c r="W189" t="s" s="2">
+        <v>565</v>
+      </c>
+      <c r="X189" t="s" s="2">
         <v>566</v>
       </c>
-      <c r="X189" t="s" s="2">
+      <c r="Y189" t="s" s="2">
         <v>567</v>
       </c>
-      <c r="Y189" t="s" s="2">
-        <v>568</v>
-      </c>
       <c r="Z189" t="s" s="2">
         <v>44</v>
       </c>
@@ -23801,7 +23797,7 @@
         <v>44</v>
       </c>
       <c r="AE189" t="s" s="2">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="AF189" t="s" s="2">
         <v>52</v>
@@ -23816,7 +23812,7 @@
         <v>44</v>
       </c>
       <c r="AJ189" t="s" s="2">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="AK189" t="s" s="2">
         <v>114</v>
@@ -23825,7 +23821,7 @@
         <v>44</v>
       </c>
       <c r="AM189" t="s" s="2">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="AN189" t="s" s="2">
         <v>44</v>
@@ -23833,7 +23829,7 @@
     </row>
     <row r="190" hidden="true">
       <c r="A190" t="s" s="2">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B190" s="2"/>
       <c r="C190" t="s" s="2">
@@ -23859,16 +23855,16 @@
         <v>207</v>
       </c>
       <c r="K190" t="s" s="2">
+        <v>570</v>
+      </c>
+      <c r="L190" t="s" s="2">
         <v>571</v>
       </c>
-      <c r="L190" t="s" s="2">
+      <c r="M190" t="s" s="2">
         <v>572</v>
       </c>
-      <c r="M190" t="s" s="2">
+      <c r="N190" t="s" s="2">
         <v>573</v>
-      </c>
-      <c r="N190" t="s" s="2">
-        <v>574</v>
       </c>
       <c r="O190" t="s" s="2">
         <v>44</v>
@@ -23893,46 +23889,46 @@
         <v>44</v>
       </c>
       <c r="W190" t="s" s="2">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="X190" t="s" s="2">
+        <v>574</v>
+      </c>
+      <c r="Y190" t="s" s="2">
         <v>575</v>
       </c>
-      <c r="Y190" t="s" s="2">
+      <c r="Z190" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA190" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB190" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC190" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD190" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE190" t="s" s="2">
+        <v>569</v>
+      </c>
+      <c r="AF190" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG190" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH190" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI190" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ190" t="s" s="2">
         <v>576</v>
-      </c>
-      <c r="Z190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE190" t="s" s="2">
-        <v>570</v>
-      </c>
-      <c r="AF190" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG190" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ190" t="s" s="2">
-        <v>577</v>
       </c>
       <c r="AK190" t="s" s="2">
         <v>114</v>
@@ -23941,7 +23937,7 @@
         <v>44</v>
       </c>
       <c r="AM190" t="s" s="2">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="AN190" t="s" s="2">
         <v>44</v>
@@ -23949,7 +23945,7 @@
     </row>
     <row r="191" hidden="true">
       <c r="A191" t="s" s="2">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B191" s="2"/>
       <c r="C191" t="s" s="2">
@@ -23975,14 +23971,14 @@
         <v>207</v>
       </c>
       <c r="K191" t="s" s="2">
+        <v>579</v>
+      </c>
+      <c r="L191" t="s" s="2">
         <v>580</v>
-      </c>
-      <c r="L191" t="s" s="2">
-        <v>581</v>
       </c>
       <c r="M191" s="2"/>
       <c r="N191" t="s" s="2">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="O191" t="s" s="2">
         <v>44</v>
@@ -24007,46 +24003,46 @@
         <v>44</v>
       </c>
       <c r="W191" t="s" s="2">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="X191" t="s" s="2">
+        <v>582</v>
+      </c>
+      <c r="Y191" t="s" s="2">
         <v>583</v>
       </c>
-      <c r="Y191" t="s" s="2">
+      <c r="Z191" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA191" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB191" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC191" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD191" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE191" t="s" s="2">
+        <v>578</v>
+      </c>
+      <c r="AF191" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG191" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH191" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI191" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ191" t="s" s="2">
         <v>584</v>
-      </c>
-      <c r="Z191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE191" t="s" s="2">
-        <v>579</v>
-      </c>
-      <c r="AF191" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG191" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ191" t="s" s="2">
-        <v>585</v>
       </c>
       <c r="AK191" t="s" s="2">
         <v>114</v>
@@ -24063,7 +24059,7 @@
     </row>
     <row r="192">
       <c r="A192" t="s" s="2">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B192" s="2"/>
       <c r="C192" t="s" s="2">
@@ -24086,19 +24082,19 @@
         <v>44</v>
       </c>
       <c r="J192" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K192" t="s" s="2">
+        <v>586</v>
+      </c>
+      <c r="L192" t="s" s="2">
         <v>587</v>
       </c>
-      <c r="L192" t="s" s="2">
+      <c r="M192" t="s" s="2">
         <v>588</v>
       </c>
-      <c r="M192" t="s" s="2">
+      <c r="N192" t="s" s="2">
         <v>589</v>
-      </c>
-      <c r="N192" t="s" s="2">
-        <v>590</v>
       </c>
       <c r="O192" t="s" s="2">
         <v>44</v>
@@ -24147,7 +24143,7 @@
         <v>44</v>
       </c>
       <c r="AE192" t="s" s="2">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="AF192" t="s" s="2">
         <v>42</v>
@@ -24159,13 +24155,13 @@
         <v>44</v>
       </c>
       <c r="AI192" t="s" s="2">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AJ192" t="s" s="2">
+        <v>590</v>
+      </c>
+      <c r="AK192" t="s" s="2">
         <v>591</v>
-      </c>
-      <c r="AK192" t="s" s="2">
-        <v>592</v>
       </c>
       <c r="AL192" t="s" s="2">
         <v>44</v>
@@ -24179,7 +24175,7 @@
     </row>
     <row r="193" hidden="true">
       <c r="A193" t="s" s="2">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B193" s="2"/>
       <c r="C193" t="s" s="2">
@@ -24291,7 +24287,7 @@
     </row>
     <row r="194" hidden="true">
       <c r="A194" t="s" s="2">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B194" s="2"/>
       <c r="C194" t="s" s="2">
@@ -24405,11 +24401,11 @@
     </row>
     <row r="195" hidden="true">
       <c r="A195" t="s" s="2">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B195" s="2"/>
       <c r="C195" t="s" s="2">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D195" s="2"/>
       <c r="E195" t="s" s="2">
@@ -24434,7 +24430,7 @@
         <v>152</v>
       </c>
       <c r="L195" t="s" s="2">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="M195" t="s" s="2">
         <v>119</v>
@@ -24487,7 +24483,7 @@
         <v>44</v>
       </c>
       <c r="AE195" t="s" s="2">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AF195" t="s" s="2">
         <v>42</v>
@@ -24519,7 +24515,7 @@
     </row>
     <row r="196">
       <c r="A196" t="s" s="2">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B196" s="2"/>
       <c r="C196" t="s" s="2">
@@ -24545,16 +24541,16 @@
         <v>207</v>
       </c>
       <c r="K196" t="s" s="2">
+        <v>596</v>
+      </c>
+      <c r="L196" t="s" s="2">
         <v>597</v>
       </c>
-      <c r="L196" t="s" s="2">
+      <c r="M196" t="s" s="2">
         <v>598</v>
       </c>
-      <c r="M196" t="s" s="2">
+      <c r="N196" t="s" s="2">
         <v>599</v>
-      </c>
-      <c r="N196" t="s" s="2">
-        <v>600</v>
       </c>
       <c r="O196" t="s" s="2">
         <v>44</v>
@@ -24583,49 +24579,49 @@
       </c>
       <c r="X196" s="2"/>
       <c r="Y196" t="s" s="2">
+        <v>600</v>
+      </c>
+      <c r="Z196" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA196" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB196" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC196" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD196" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE196" t="s" s="2">
+        <v>595</v>
+      </c>
+      <c r="AF196" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AG196" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH196" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI196" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ196" t="s" s="2">
         <v>601</v>
       </c>
-      <c r="Z196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE196" t="s" s="2">
-        <v>596</v>
-      </c>
-      <c r="AF196" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AG196" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ196" t="s" s="2">
+      <c r="AK196" t="s" s="2">
         <v>602</v>
       </c>
-      <c r="AK196" t="s" s="2">
+      <c r="AL196" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM196" t="s" s="2">
         <v>603</v>
-      </c>
-      <c r="AL196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM196" t="s" s="2">
-        <v>604</v>
       </c>
       <c r="AN196" t="s" s="2">
         <v>44</v>
@@ -24633,7 +24629,7 @@
     </row>
     <row r="197">
       <c r="A197" t="s" s="2">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B197" s="2"/>
       <c r="C197" t="s" s="2">
@@ -24659,16 +24655,16 @@
         <v>381</v>
       </c>
       <c r="K197" t="s" s="2">
+        <v>605</v>
+      </c>
+      <c r="L197" t="s" s="2">
         <v>606</v>
       </c>
-      <c r="L197" t="s" s="2">
+      <c r="M197" t="s" s="2">
         <v>607</v>
       </c>
-      <c r="M197" t="s" s="2">
+      <c r="N197" t="s" s="2">
         <v>608</v>
-      </c>
-      <c r="N197" t="s" s="2">
-        <v>609</v>
       </c>
       <c r="O197" t="s" s="2">
         <v>44</v>
@@ -24717,7 +24713,7 @@
         <v>44</v>
       </c>
       <c r="AE197" t="s" s="2">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AF197" t="s" s="2">
         <v>42</v>
@@ -24732,16 +24728,16 @@
         <v>44</v>
       </c>
       <c r="AJ197" t="s" s="2">
+        <v>609</v>
+      </c>
+      <c r="AK197" t="s" s="2">
         <v>610</v>
       </c>
-      <c r="AK197" t="s" s="2">
+      <c r="AL197" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM197" t="s" s="2">
         <v>611</v>
-      </c>
-      <c r="AL197" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM197" t="s" s="2">
-        <v>612</v>
       </c>
       <c r="AN197" t="s" s="2">
         <v>44</v>
@@ -24749,14 +24745,14 @@
     </row>
     <row r="198">
       <c r="A198" t="s" s="2">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B198" s="2"/>
       <c r="C198" t="s" s="2">
+        <v>613</v>
+      </c>
+      <c r="D198" t="s" s="2">
         <v>614</v>
-      </c>
-      <c r="D198" t="s" s="2">
-        <v>615</v>
       </c>
       <c r="E198" t="s" s="2">
         <v>42</v>
@@ -24774,16 +24770,16 @@
         <v>44</v>
       </c>
       <c r="J198" t="s" s="2">
+        <v>615</v>
+      </c>
+      <c r="K198" t="s" s="2">
         <v>616</v>
       </c>
-      <c r="K198" t="s" s="2">
+      <c r="L198" t="s" s="2">
         <v>617</v>
       </c>
-      <c r="L198" t="s" s="2">
+      <c r="M198" t="s" s="2">
         <v>618</v>
-      </c>
-      <c r="M198" t="s" s="2">
-        <v>619</v>
       </c>
       <c r="N198" s="2"/>
       <c r="O198" t="s" s="2">
@@ -24833,7 +24829,7 @@
         <v>44</v>
       </c>
       <c r="AE198" t="s" s="2">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AF198" t="s" s="2">
         <v>42</v>
@@ -24848,7 +24844,7 @@
         <v>44</v>
       </c>
       <c r="AJ198" t="s" s="2">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="AK198" t="s" s="2">
         <v>114</v>
@@ -24857,7 +24853,7 @@
         <v>44</v>
       </c>
       <c r="AM198" t="s" s="2">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AN198" t="s" s="2">
         <v>44</v>
@@ -24865,14 +24861,14 @@
     </row>
     <row r="199">
       <c r="A199" t="s" s="2">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B199" s="2"/>
       <c r="C199" t="s" s="2">
         <v>44</v>
       </c>
       <c r="D199" t="s" s="2">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E199" t="s" s="2">
         <v>42</v>
@@ -24890,19 +24886,19 @@
         <v>53</v>
       </c>
       <c r="J199" t="s" s="2">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K199" t="s" s="2">
+        <v>623</v>
+      </c>
+      <c r="L199" t="s" s="2">
         <v>624</v>
       </c>
-      <c r="L199" t="s" s="2">
+      <c r="M199" t="s" s="2">
         <v>625</v>
       </c>
-      <c r="M199" t="s" s="2">
+      <c r="N199" t="s" s="2">
         <v>626</v>
-      </c>
-      <c r="N199" t="s" s="2">
-        <v>627</v>
       </c>
       <c r="O199" t="s" s="2">
         <v>44</v>
@@ -24951,7 +24947,7 @@
         <v>44</v>
       </c>
       <c r="AE199" t="s" s="2">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="AF199" t="s" s="2">
         <v>42</v>
@@ -24966,10 +24962,10 @@
         <v>44</v>
       </c>
       <c r="AJ199" t="s" s="2">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="AK199" t="s" s="2">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="AL199" t="s" s="2">
         <v>44</v>
@@ -24983,7 +24979,7 @@
     </row>
     <row r="200" hidden="true">
       <c r="A200" t="s" s="2">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B200" s="2"/>
       <c r="C200" t="s" s="2">
@@ -25006,19 +25002,19 @@
         <v>53</v>
       </c>
       <c r="J200" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K200" t="s" s="2">
+        <v>629</v>
+      </c>
+      <c r="L200" t="s" s="2">
         <v>630</v>
       </c>
-      <c r="L200" t="s" s="2">
+      <c r="M200" t="s" s="2">
         <v>631</v>
       </c>
-      <c r="M200" t="s" s="2">
+      <c r="N200" t="s" s="2">
         <v>632</v>
-      </c>
-      <c r="N200" t="s" s="2">
-        <v>633</v>
       </c>
       <c r="O200" t="s" s="2">
         <v>44</v>
@@ -25067,7 +25063,7 @@
         <v>44</v>
       </c>
       <c r="AE200" t="s" s="2">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AF200" t="s" s="2">
         <v>42</v>
@@ -25079,10 +25075,10 @@
         <v>44</v>
       </c>
       <c r="AI200" t="s" s="2">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AJ200" t="s" s="2">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="AK200" t="s" s="2">
         <v>114</v>
@@ -25099,7 +25095,7 @@
     </row>
     <row r="201" hidden="true">
       <c r="A201" t="s" s="2">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B201" s="2"/>
       <c r="C201" t="s" s="2">
@@ -25211,7 +25207,7 @@
     </row>
     <row r="202" hidden="true">
       <c r="A202" t="s" s="2">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B202" s="2"/>
       <c r="C202" t="s" s="2">
@@ -25325,11 +25321,11 @@
     </row>
     <row r="203" hidden="true">
       <c r="A203" t="s" s="2">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B203" s="2"/>
       <c r="C203" t="s" s="2">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D203" s="2"/>
       <c r="E203" t="s" s="2">
@@ -25354,7 +25350,7 @@
         <v>152</v>
       </c>
       <c r="L203" t="s" s="2">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="M203" t="s" s="2">
         <v>119</v>
@@ -25407,7 +25403,7 @@
         <v>44</v>
       </c>
       <c r="AE203" t="s" s="2">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AF203" t="s" s="2">
         <v>42</v>
@@ -25439,7 +25435,7 @@
     </row>
     <row r="204" hidden="true">
       <c r="A204" t="s" s="2">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B204" s="2"/>
       <c r="C204" t="s" s="2">
@@ -25462,16 +25458,16 @@
         <v>53</v>
       </c>
       <c r="J204" t="s" s="2">
+        <v>638</v>
+      </c>
+      <c r="K204" t="s" s="2">
         <v>639</v>
       </c>
-      <c r="K204" t="s" s="2">
+      <c r="L204" t="s" s="2">
         <v>640</v>
       </c>
-      <c r="L204" t="s" s="2">
+      <c r="M204" t="s" s="2">
         <v>641</v>
-      </c>
-      <c r="M204" t="s" s="2">
-        <v>642</v>
       </c>
       <c r="N204" s="2"/>
       <c r="O204" t="s" s="2">
@@ -25521,7 +25517,7 @@
         <v>44</v>
       </c>
       <c r="AE204" t="s" s="2">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="AF204" t="s" s="2">
         <v>52</v>
@@ -25545,7 +25541,7 @@
         <v>44</v>
       </c>
       <c r="AM204" t="s" s="2">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AN204" t="s" s="2">
         <v>44</v>
@@ -25553,7 +25549,7 @@
     </row>
     <row r="205" hidden="true">
       <c r="A205" t="s" s="2">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B205" s="2"/>
       <c r="C205" t="s" s="2">
@@ -25579,10 +25575,10 @@
         <v>71</v>
       </c>
       <c r="K205" t="s" s="2">
+        <v>644</v>
+      </c>
+      <c r="L205" t="s" s="2">
         <v>645</v>
-      </c>
-      <c r="L205" t="s" s="2">
-        <v>646</v>
       </c>
       <c r="M205" s="2"/>
       <c r="N205" s="2"/>
@@ -25612,43 +25608,43 @@
         <v>185</v>
       </c>
       <c r="X205" t="s" s="2">
+        <v>645</v>
+      </c>
+      <c r="Y205" t="s" s="2">
         <v>646</v>
       </c>
-      <c r="Y205" t="s" s="2">
+      <c r="Z205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE205" t="s" s="2">
+        <v>643</v>
+      </c>
+      <c r="AF205" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AG205" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ205" t="s" s="2">
         <v>647</v>
-      </c>
-      <c r="Z205" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA205" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB205" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC205" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD205" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE205" t="s" s="2">
-        <v>644</v>
-      </c>
-      <c r="AF205" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AG205" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH205" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI205" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ205" t="s" s="2">
-        <v>648</v>
       </c>
       <c r="AK205" t="s" s="2">
         <v>114</v>

</xml_diff>

<commit_message>
Saved newly generated CDA IGs for following FHIR documents
Shared HealthSummary
Event Summary
Personal Health Records
Prescription and Dispense Lists
Advance Care Records
Shared Medicines List
</commit_message>
<xml_diff>
--- a/output/AdvanceCareRecords/patient-dh-base-1.xlsx
+++ b/output/AdvanceCareRecords/patient-dh-base-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7395" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7395" uniqueCount="649">
   <si>
     <t>Path</t>
   </si>
@@ -1439,6 +1439,10 @@
   </si>
   <si>
     <t>Patient.birthDate.value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
   </si>
   <si>
     <t>Primitive value for date</t>
@@ -20654,13 +20658,13 @@
         <v>44</v>
       </c>
       <c r="J162" t="s" s="2">
-        <v>419</v>
+        <v>447</v>
       </c>
       <c r="K162" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="L162" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="M162" s="2"/>
       <c r="N162" s="2"/>
@@ -20711,7 +20715,7 @@
         <v>44</v>
       </c>
       <c r="AE162" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AF162" t="s" s="2">
         <v>42</v>
@@ -20743,7 +20747,7 @@
     </row>
     <row r="163" hidden="true">
       <c r="A163" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" t="s" s="2">
@@ -20766,19 +20770,19 @@
         <v>53</v>
       </c>
       <c r="J163" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="K163" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="L163" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="M163" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="N163" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="O163" t="s" s="2">
         <v>44</v>
@@ -20825,7 +20829,7 @@
         <v>182</v>
       </c>
       <c r="AE163" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AF163" t="s" s="2">
         <v>42</v>
@@ -20840,7 +20844,7 @@
         <v>44</v>
       </c>
       <c r="AJ163" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AK163" t="s" s="2">
         <v>114</v>
@@ -20849,7 +20853,7 @@
         <v>44</v>
       </c>
       <c r="AM163" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="AN163" t="s" s="2">
         <v>44</v>
@@ -20857,10 +20861,10 @@
     </row>
     <row r="164">
       <c r="A164" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B164" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C164" t="s" s="2">
         <v>44</v>
@@ -20885,16 +20889,16 @@
         <v>381</v>
       </c>
       <c r="K164" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="L164" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="M164" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="N164" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="O164" t="s" s="2">
         <v>44</v>
@@ -20943,7 +20947,7 @@
         <v>44</v>
       </c>
       <c r="AE164" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AF164" t="s" s="2">
         <v>42</v>
@@ -20958,7 +20962,7 @@
         <v>44</v>
       </c>
       <c r="AJ164" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AK164" t="s" s="2">
         <v>114</v>
@@ -20967,7 +20971,7 @@
         <v>44</v>
       </c>
       <c r="AM164" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="AN164" t="s" s="2">
         <v>44</v>
@@ -20975,10 +20979,10 @@
     </row>
     <row r="165">
       <c r="A165" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B165" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C165" t="s" s="2">
         <v>44</v>
@@ -21003,16 +21007,16 @@
         <v>286</v>
       </c>
       <c r="K165" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="L165" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="M165" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="N165" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="O165" t="s" s="2">
         <v>44</v>
@@ -21061,7 +21065,7 @@
         <v>44</v>
       </c>
       <c r="AE165" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AF165" t="s" s="2">
         <v>42</v>
@@ -21076,7 +21080,7 @@
         <v>44</v>
       </c>
       <c r="AJ165" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AK165" t="s" s="2">
         <v>114</v>
@@ -21085,7 +21089,7 @@
         <v>44</v>
       </c>
       <c r="AM165" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="AN165" t="s" s="2">
         <v>44</v>
@@ -21093,7 +21097,7 @@
     </row>
     <row r="166" hidden="true">
       <c r="A166" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B166" s="2"/>
       <c r="C166" t="s" s="2">
@@ -21205,7 +21209,7 @@
     </row>
     <row r="167" hidden="true">
       <c r="A167" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B167" s="2"/>
       <c r="C167" t="s" s="2">
@@ -21315,7 +21319,7 @@
     </row>
     <row r="168">
       <c r="A168" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B168" t="s" s="2">
         <v>431</v>
@@ -21431,7 +21435,7 @@
     </row>
     <row r="169" hidden="true">
       <c r="A169" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B169" s="2"/>
       <c r="C169" t="s" s="2">
@@ -21454,13 +21458,13 @@
         <v>44</v>
       </c>
       <c r="J169" t="s" s="2">
-        <v>286</v>
+        <v>447</v>
       </c>
       <c r="K169" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="L169" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="M169" s="2"/>
       <c r="N169" s="2"/>
@@ -21511,7 +21515,7 @@
         <v>44</v>
       </c>
       <c r="AE169" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AF169" t="s" s="2">
         <v>42</v>
@@ -21543,7 +21547,7 @@
     </row>
     <row r="170">
       <c r="A170" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B170" s="2"/>
       <c r="C170" t="s" s="2">
@@ -21569,16 +21573,16 @@
         <v>130</v>
       </c>
       <c r="K170" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="L170" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="M170" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="N170" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="O170" t="s" s="2">
         <v>44</v>
@@ -21627,7 +21631,7 @@
         <v>44</v>
       </c>
       <c r="AE170" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="AF170" t="s" s="2">
         <v>42</v>
@@ -21642,16 +21646,16 @@
         <v>44</v>
       </c>
       <c r="AJ170" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="AK170" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="AL170" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM170" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="AN170" t="s" s="2">
         <v>44</v>
@@ -21659,7 +21663,7 @@
     </row>
     <row r="171">
       <c r="A171" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B171" s="2"/>
       <c r="C171" t="s" s="2">
@@ -21685,14 +21689,14 @@
         <v>207</v>
       </c>
       <c r="K171" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="L171" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="M171" s="2"/>
       <c r="N171" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="O171" t="s" s="2">
         <v>44</v>
@@ -21720,10 +21724,10 @@
         <v>75</v>
       </c>
       <c r="X171" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="Y171" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="Z171" t="s" s="2">
         <v>44</v>
@@ -21741,7 +21745,7 @@
         <v>44</v>
       </c>
       <c r="AE171" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AF171" t="s" s="2">
         <v>42</v>
@@ -21756,16 +21760,16 @@
         <v>44</v>
       </c>
       <c r="AJ171" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="AK171" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="AL171" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM171" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="AN171" t="s" s="2">
         <v>44</v>
@@ -21773,7 +21777,7 @@
     </row>
     <row r="172">
       <c r="A172" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B172" s="2"/>
       <c r="C172" t="s" s="2">
@@ -21796,19 +21800,19 @@
         <v>44</v>
       </c>
       <c r="J172" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="K172" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="L172" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="M172" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="N172" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="O172" t="s" s="2">
         <v>44</v>
@@ -21857,7 +21861,7 @@
         <v>44</v>
       </c>
       <c r="AE172" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="AF172" t="s" s="2">
         <v>42</v>
@@ -21872,7 +21876,7 @@
         <v>44</v>
       </c>
       <c r="AJ172" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="AK172" t="s" s="2">
         <v>114</v>
@@ -21881,7 +21885,7 @@
         <v>44</v>
       </c>
       <c r="AM172" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="AN172" t="s" s="2">
         <v>44</v>
@@ -21889,7 +21893,7 @@
     </row>
     <row r="173" hidden="true">
       <c r="A173" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B173" s="2"/>
       <c r="C173" t="s" s="2">
@@ -21912,17 +21916,17 @@
         <v>44</v>
       </c>
       <c r="J173" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="K173" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="L173" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="M173" s="2"/>
       <c r="N173" t="s" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="O173" t="s" s="2">
         <v>44</v>
@@ -21971,7 +21975,7 @@
         <v>44</v>
       </c>
       <c r="AE173" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="AF173" t="s" s="2">
         <v>42</v>
@@ -21986,7 +21990,7 @@
         <v>44</v>
       </c>
       <c r="AJ173" t="s" s="2">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="AK173" t="s" s="2">
         <v>114</v>
@@ -21995,7 +21999,7 @@
         <v>44</v>
       </c>
       <c r="AM173" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="AN173" t="s" s="2">
         <v>44</v>
@@ -22003,7 +22007,7 @@
     </row>
     <row r="174">
       <c r="A174" t="s" s="2">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B174" s="2"/>
       <c r="C174" t="s" s="2">
@@ -22026,19 +22030,19 @@
         <v>44</v>
       </c>
       <c r="J174" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="K174" t="s" s="2">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="L174" t="s" s="2">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="M174" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="N174" t="s" s="2">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="O174" t="s" s="2">
         <v>44</v>
@@ -22087,7 +22091,7 @@
         <v>44</v>
       </c>
       <c r="AE174" t="s" s="2">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="AF174" t="s" s="2">
         <v>42</v>
@@ -22099,10 +22103,10 @@
         <v>44</v>
       </c>
       <c r="AI174" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="AJ174" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="AK174" t="s" s="2">
         <v>114</v>
@@ -22119,7 +22123,7 @@
     </row>
     <row r="175" hidden="true">
       <c r="A175" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B175" s="2"/>
       <c r="C175" t="s" s="2">
@@ -22231,7 +22235,7 @@
     </row>
     <row r="176" hidden="true">
       <c r="A176" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B176" s="2"/>
       <c r="C176" t="s" s="2">
@@ -22345,11 +22349,11 @@
     </row>
     <row r="177" hidden="true">
       <c r="A177" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B177" s="2"/>
       <c r="C177" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D177" s="2"/>
       <c r="E177" t="s" s="2">
@@ -22374,7 +22378,7 @@
         <v>152</v>
       </c>
       <c r="L177" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="M177" t="s" s="2">
         <v>119</v>
@@ -22427,7 +22431,7 @@
         <v>44</v>
       </c>
       <c r="AE177" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="AF177" t="s" s="2">
         <v>42</v>
@@ -22459,7 +22463,7 @@
     </row>
     <row r="178">
       <c r="A178" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B178" s="2"/>
       <c r="C178" t="s" s="2">
@@ -22485,14 +22489,14 @@
         <v>207</v>
       </c>
       <c r="K178" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="L178" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="M178" s="2"/>
       <c r="N178" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="O178" t="s" s="2">
         <v>44</v>
@@ -22521,7 +22525,7 @@
       </c>
       <c r="X178" s="2"/>
       <c r="Y178" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="Z178" t="s" s="2">
         <v>44</v>
@@ -22539,7 +22543,7 @@
         <v>44</v>
       </c>
       <c r="AE178" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="AF178" t="s" s="2">
         <v>42</v>
@@ -22554,7 +22558,7 @@
         <v>44</v>
       </c>
       <c r="AJ178" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="AK178" t="s" s="2">
         <v>114</v>
@@ -22563,7 +22567,7 @@
         <v>44</v>
       </c>
       <c r="AM178" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="AN178" t="s" s="2">
         <v>44</v>
@@ -22571,7 +22575,7 @@
     </row>
     <row r="179">
       <c r="A179" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B179" s="2"/>
       <c r="C179" t="s" s="2">
@@ -22606,7 +22610,7 @@
         <v>393</v>
       </c>
       <c r="N179" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="O179" t="s" s="2">
         <v>44</v>
@@ -22655,7 +22659,7 @@
         <v>44</v>
       </c>
       <c r="AE179" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="AF179" t="s" s="2">
         <v>42</v>
@@ -22687,7 +22691,7 @@
     </row>
     <row r="180">
       <c r="A180" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B180" s="2"/>
       <c r="C180" t="s" s="2">
@@ -22713,13 +22717,13 @@
         <v>399</v>
       </c>
       <c r="K180" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="L180" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="M180" t="s" s="2">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="N180" t="s" s="2">
         <v>403</v>
@@ -22771,7 +22775,7 @@
         <v>44</v>
       </c>
       <c r="AE180" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="AF180" t="s" s="2">
         <v>42</v>
@@ -22795,7 +22799,7 @@
         <v>44</v>
       </c>
       <c r="AM180" t="s" s="2">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="AN180" t="s" s="2">
         <v>44</v>
@@ -22803,7 +22807,7 @@
     </row>
     <row r="181">
       <c r="A181" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B181" s="2"/>
       <c r="C181" t="s" s="2">
@@ -22829,14 +22833,14 @@
         <v>130</v>
       </c>
       <c r="K181" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="L181" t="s" s="2">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="M181" s="2"/>
       <c r="N181" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="O181" t="s" s="2">
         <v>44</v>
@@ -22885,7 +22889,7 @@
         <v>44</v>
       </c>
       <c r="AE181" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="AF181" t="s" s="2">
         <v>42</v>
@@ -22900,7 +22904,7 @@
         <v>44</v>
       </c>
       <c r="AJ181" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="AK181" t="s" s="2">
         <v>114</v>
@@ -22909,7 +22913,7 @@
         <v>44</v>
       </c>
       <c r="AM181" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="AN181" t="s" s="2">
         <v>44</v>
@@ -22917,7 +22921,7 @@
     </row>
     <row r="182">
       <c r="A182" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B182" s="2"/>
       <c r="C182" t="s" s="2">
@@ -22946,11 +22950,11 @@
         <v>408</v>
       </c>
       <c r="L182" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="M182" s="2"/>
       <c r="N182" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="O182" t="s" s="2">
         <v>44</v>
@@ -22999,7 +23003,7 @@
         <v>44</v>
       </c>
       <c r="AE182" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="AF182" t="s" s="2">
         <v>42</v>
@@ -23023,7 +23027,7 @@
         <v>44</v>
       </c>
       <c r="AM182" t="s" s="2">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="AN182" t="s" s="2">
         <v>44</v>
@@ -23031,7 +23035,7 @@
     </row>
     <row r="183">
       <c r="A183" t="s" s="2">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B183" s="2"/>
       <c r="C183" t="s" s="2">
@@ -23054,17 +23058,17 @@
         <v>44</v>
       </c>
       <c r="J183" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="K183" t="s" s="2">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="L183" t="s" s="2">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="M183" s="2"/>
       <c r="N183" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="O183" t="s" s="2">
         <v>44</v>
@@ -23113,7 +23117,7 @@
         <v>44</v>
       </c>
       <c r="AE183" t="s" s="2">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="AF183" t="s" s="2">
         <v>42</v>
@@ -23122,13 +23126,13 @@
         <v>52</v>
       </c>
       <c r="AH183" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="AI183" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AJ183" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="AK183" t="s" s="2">
         <v>114</v>
@@ -23137,7 +23141,7 @@
         <v>44</v>
       </c>
       <c r="AM183" t="s" s="2">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="AN183" t="s" s="2">
         <v>44</v>
@@ -23145,7 +23149,7 @@
     </row>
     <row r="184">
       <c r="A184" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B184" s="2"/>
       <c r="C184" t="s" s="2">
@@ -23171,10 +23175,10 @@
         <v>255</v>
       </c>
       <c r="K184" t="s" s="2">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="L184" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="M184" s="2"/>
       <c r="N184" s="2"/>
@@ -23225,7 +23229,7 @@
         <v>44</v>
       </c>
       <c r="AE184" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="AF184" t="s" s="2">
         <v>42</v>
@@ -23240,7 +23244,7 @@
         <v>44</v>
       </c>
       <c r="AJ184" t="s" s="2">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="AK184" t="s" s="2">
         <v>114</v>
@@ -23257,7 +23261,7 @@
     </row>
     <row r="185" hidden="true">
       <c r="A185" t="s" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B185" s="2"/>
       <c r="C185" t="s" s="2">
@@ -23280,19 +23284,19 @@
         <v>53</v>
       </c>
       <c r="J185" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="K185" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="L185" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="M185" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="N185" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="O185" t="s" s="2">
         <v>44</v>
@@ -23341,7 +23345,7 @@
         <v>44</v>
       </c>
       <c r="AE185" t="s" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="AF185" t="s" s="2">
         <v>42</v>
@@ -23353,10 +23357,10 @@
         <v>44</v>
       </c>
       <c r="AI185" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="AJ185" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="AK185" t="s" s="2">
         <v>114</v>
@@ -23373,7 +23377,7 @@
     </row>
     <row r="186" hidden="true">
       <c r="A186" t="s" s="2">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B186" s="2"/>
       <c r="C186" t="s" s="2">
@@ -23485,7 +23489,7 @@
     </row>
     <row r="187" hidden="true">
       <c r="A187" t="s" s="2">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B187" s="2"/>
       <c r="C187" t="s" s="2">
@@ -23599,11 +23603,11 @@
     </row>
     <row r="188" hidden="true">
       <c r="A188" t="s" s="2">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B188" s="2"/>
       <c r="C188" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D188" s="2"/>
       <c r="E188" t="s" s="2">
@@ -23628,7 +23632,7 @@
         <v>152</v>
       </c>
       <c r="L188" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="M188" t="s" s="2">
         <v>119</v>
@@ -23681,7 +23685,7 @@
         <v>44</v>
       </c>
       <c r="AE188" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="AF188" t="s" s="2">
         <v>42</v>
@@ -23713,7 +23717,7 @@
     </row>
     <row r="189" hidden="true">
       <c r="A189" t="s" s="2">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B189" s="2"/>
       <c r="C189" t="s" s="2">
@@ -23739,16 +23743,16 @@
         <v>207</v>
       </c>
       <c r="K189" t="s" s="2">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="L189" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="M189" t="s" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="N189" t="s" s="2">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="O189" t="s" s="2">
         <v>44</v>
@@ -23773,13 +23777,13 @@
         <v>44</v>
       </c>
       <c r="W189" t="s" s="2">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="X189" t="s" s="2">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="Y189" t="s" s="2">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="Z189" t="s" s="2">
         <v>44</v>
@@ -23797,7 +23801,7 @@
         <v>44</v>
       </c>
       <c r="AE189" t="s" s="2">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="AF189" t="s" s="2">
         <v>52</v>
@@ -23812,7 +23816,7 @@
         <v>44</v>
       </c>
       <c r="AJ189" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="AK189" t="s" s="2">
         <v>114</v>
@@ -23821,7 +23825,7 @@
         <v>44</v>
       </c>
       <c r="AM189" t="s" s="2">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="AN189" t="s" s="2">
         <v>44</v>
@@ -23829,7 +23833,7 @@
     </row>
     <row r="190" hidden="true">
       <c r="A190" t="s" s="2">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B190" s="2"/>
       <c r="C190" t="s" s="2">
@@ -23855,16 +23859,16 @@
         <v>207</v>
       </c>
       <c r="K190" t="s" s="2">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="L190" t="s" s="2">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="M190" t="s" s="2">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="N190" t="s" s="2">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="O190" t="s" s="2">
         <v>44</v>
@@ -23889,13 +23893,13 @@
         <v>44</v>
       </c>
       <c r="W190" t="s" s="2">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="X190" t="s" s="2">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="Y190" t="s" s="2">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="Z190" t="s" s="2">
         <v>44</v>
@@ -23913,7 +23917,7 @@
         <v>44</v>
       </c>
       <c r="AE190" t="s" s="2">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="AF190" t="s" s="2">
         <v>42</v>
@@ -23928,7 +23932,7 @@
         <v>44</v>
       </c>
       <c r="AJ190" t="s" s="2">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="AK190" t="s" s="2">
         <v>114</v>
@@ -23937,7 +23941,7 @@
         <v>44</v>
       </c>
       <c r="AM190" t="s" s="2">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="AN190" t="s" s="2">
         <v>44</v>
@@ -23945,7 +23949,7 @@
     </row>
     <row r="191" hidden="true">
       <c r="A191" t="s" s="2">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B191" s="2"/>
       <c r="C191" t="s" s="2">
@@ -23971,14 +23975,14 @@
         <v>207</v>
       </c>
       <c r="K191" t="s" s="2">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="L191" t="s" s="2">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="M191" s="2"/>
       <c r="N191" t="s" s="2">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="O191" t="s" s="2">
         <v>44</v>
@@ -24003,13 +24007,13 @@
         <v>44</v>
       </c>
       <c r="W191" t="s" s="2">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="X191" t="s" s="2">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="Y191" t="s" s="2">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="Z191" t="s" s="2">
         <v>44</v>
@@ -24027,7 +24031,7 @@
         <v>44</v>
       </c>
       <c r="AE191" t="s" s="2">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="AF191" t="s" s="2">
         <v>42</v>
@@ -24042,7 +24046,7 @@
         <v>44</v>
       </c>
       <c r="AJ191" t="s" s="2">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="AK191" t="s" s="2">
         <v>114</v>
@@ -24059,7 +24063,7 @@
     </row>
     <row r="192">
       <c r="A192" t="s" s="2">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B192" s="2"/>
       <c r="C192" t="s" s="2">
@@ -24082,19 +24086,19 @@
         <v>44</v>
       </c>
       <c r="J192" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="K192" t="s" s="2">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="L192" t="s" s="2">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="M192" t="s" s="2">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="N192" t="s" s="2">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="O192" t="s" s="2">
         <v>44</v>
@@ -24143,7 +24147,7 @@
         <v>44</v>
       </c>
       <c r="AE192" t="s" s="2">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="AF192" t="s" s="2">
         <v>42</v>
@@ -24155,13 +24159,13 @@
         <v>44</v>
       </c>
       <c r="AI192" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="AJ192" t="s" s="2">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="AK192" t="s" s="2">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="AL192" t="s" s="2">
         <v>44</v>
@@ -24175,7 +24179,7 @@
     </row>
     <row r="193" hidden="true">
       <c r="A193" t="s" s="2">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B193" s="2"/>
       <c r="C193" t="s" s="2">
@@ -24287,7 +24291,7 @@
     </row>
     <row r="194" hidden="true">
       <c r="A194" t="s" s="2">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B194" s="2"/>
       <c r="C194" t="s" s="2">
@@ -24401,11 +24405,11 @@
     </row>
     <row r="195" hidden="true">
       <c r="A195" t="s" s="2">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B195" s="2"/>
       <c r="C195" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D195" s="2"/>
       <c r="E195" t="s" s="2">
@@ -24430,7 +24434,7 @@
         <v>152</v>
       </c>
       <c r="L195" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="M195" t="s" s="2">
         <v>119</v>
@@ -24483,7 +24487,7 @@
         <v>44</v>
       </c>
       <c r="AE195" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="AF195" t="s" s="2">
         <v>42</v>
@@ -24515,7 +24519,7 @@
     </row>
     <row r="196">
       <c r="A196" t="s" s="2">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B196" s="2"/>
       <c r="C196" t="s" s="2">
@@ -24541,16 +24545,16 @@
         <v>207</v>
       </c>
       <c r="K196" t="s" s="2">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="L196" t="s" s="2">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="M196" t="s" s="2">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="N196" t="s" s="2">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="O196" t="s" s="2">
         <v>44</v>
@@ -24579,7 +24583,7 @@
       </c>
       <c r="X196" s="2"/>
       <c r="Y196" t="s" s="2">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="Z196" t="s" s="2">
         <v>44</v>
@@ -24597,7 +24601,7 @@
         <v>44</v>
       </c>
       <c r="AE196" t="s" s="2">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="AF196" t="s" s="2">
         <v>52</v>
@@ -24612,16 +24616,16 @@
         <v>44</v>
       </c>
       <c r="AJ196" t="s" s="2">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="AK196" t="s" s="2">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="AL196" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM196" t="s" s="2">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="AN196" t="s" s="2">
         <v>44</v>
@@ -24629,7 +24633,7 @@
     </row>
     <row r="197">
       <c r="A197" t="s" s="2">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B197" s="2"/>
       <c r="C197" t="s" s="2">
@@ -24655,16 +24659,16 @@
         <v>381</v>
       </c>
       <c r="K197" t="s" s="2">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="L197" t="s" s="2">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="M197" t="s" s="2">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="N197" t="s" s="2">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="O197" t="s" s="2">
         <v>44</v>
@@ -24713,7 +24717,7 @@
         <v>44</v>
       </c>
       <c r="AE197" t="s" s="2">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="AF197" t="s" s="2">
         <v>42</v>
@@ -24728,16 +24732,16 @@
         <v>44</v>
       </c>
       <c r="AJ197" t="s" s="2">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="AK197" t="s" s="2">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="AL197" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM197" t="s" s="2">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="AN197" t="s" s="2">
         <v>44</v>
@@ -24745,14 +24749,14 @@
     </row>
     <row r="198">
       <c r="A198" t="s" s="2">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B198" s="2"/>
       <c r="C198" t="s" s="2">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D198" t="s" s="2">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="E198" t="s" s="2">
         <v>42</v>
@@ -24770,16 +24774,16 @@
         <v>44</v>
       </c>
       <c r="J198" t="s" s="2">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="K198" t="s" s="2">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="L198" t="s" s="2">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="M198" t="s" s="2">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="N198" s="2"/>
       <c r="O198" t="s" s="2">
@@ -24829,7 +24833,7 @@
         <v>44</v>
       </c>
       <c r="AE198" t="s" s="2">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="AF198" t="s" s="2">
         <v>42</v>
@@ -24844,7 +24848,7 @@
         <v>44</v>
       </c>
       <c r="AJ198" t="s" s="2">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="AK198" t="s" s="2">
         <v>114</v>
@@ -24853,7 +24857,7 @@
         <v>44</v>
       </c>
       <c r="AM198" t="s" s="2">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="AN198" t="s" s="2">
         <v>44</v>
@@ -24861,14 +24865,14 @@
     </row>
     <row r="199">
       <c r="A199" t="s" s="2">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B199" s="2"/>
       <c r="C199" t="s" s="2">
         <v>44</v>
       </c>
       <c r="D199" t="s" s="2">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="E199" t="s" s="2">
         <v>42</v>
@@ -24886,19 +24890,19 @@
         <v>53</v>
       </c>
       <c r="J199" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="K199" t="s" s="2">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="L199" t="s" s="2">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="M199" t="s" s="2">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="N199" t="s" s="2">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="O199" t="s" s="2">
         <v>44</v>
@@ -24947,7 +24951,7 @@
         <v>44</v>
       </c>
       <c r="AE199" t="s" s="2">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="AF199" t="s" s="2">
         <v>42</v>
@@ -24962,10 +24966,10 @@
         <v>44</v>
       </c>
       <c r="AJ199" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="AK199" t="s" s="2">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="AL199" t="s" s="2">
         <v>44</v>
@@ -24979,7 +24983,7 @@
     </row>
     <row r="200" hidden="true">
       <c r="A200" t="s" s="2">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B200" s="2"/>
       <c r="C200" t="s" s="2">
@@ -25002,19 +25006,19 @@
         <v>53</v>
       </c>
       <c r="J200" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="K200" t="s" s="2">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="L200" t="s" s="2">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="M200" t="s" s="2">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="N200" t="s" s="2">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="O200" t="s" s="2">
         <v>44</v>
@@ -25063,7 +25067,7 @@
         <v>44</v>
       </c>
       <c r="AE200" t="s" s="2">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="AF200" t="s" s="2">
         <v>42</v>
@@ -25075,10 +25079,10 @@
         <v>44</v>
       </c>
       <c r="AI200" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="AJ200" t="s" s="2">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="AK200" t="s" s="2">
         <v>114</v>
@@ -25095,7 +25099,7 @@
     </row>
     <row r="201" hidden="true">
       <c r="A201" t="s" s="2">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B201" s="2"/>
       <c r="C201" t="s" s="2">
@@ -25207,7 +25211,7 @@
     </row>
     <row r="202" hidden="true">
       <c r="A202" t="s" s="2">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B202" s="2"/>
       <c r="C202" t="s" s="2">
@@ -25321,11 +25325,11 @@
     </row>
     <row r="203" hidden="true">
       <c r="A203" t="s" s="2">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="B203" s="2"/>
       <c r="C203" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D203" s="2"/>
       <c r="E203" t="s" s="2">
@@ -25350,7 +25354,7 @@
         <v>152</v>
       </c>
       <c r="L203" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="M203" t="s" s="2">
         <v>119</v>
@@ -25403,7 +25407,7 @@
         <v>44</v>
       </c>
       <c r="AE203" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="AF203" t="s" s="2">
         <v>42</v>
@@ -25435,7 +25439,7 @@
     </row>
     <row r="204" hidden="true">
       <c r="A204" t="s" s="2">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B204" s="2"/>
       <c r="C204" t="s" s="2">
@@ -25458,16 +25462,16 @@
         <v>53</v>
       </c>
       <c r="J204" t="s" s="2">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="K204" t="s" s="2">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="L204" t="s" s="2">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="M204" t="s" s="2">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="N204" s="2"/>
       <c r="O204" t="s" s="2">
@@ -25517,7 +25521,7 @@
         <v>44</v>
       </c>
       <c r="AE204" t="s" s="2">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="AF204" t="s" s="2">
         <v>52</v>
@@ -25541,7 +25545,7 @@
         <v>44</v>
       </c>
       <c r="AM204" t="s" s="2">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="AN204" t="s" s="2">
         <v>44</v>
@@ -25549,7 +25553,7 @@
     </row>
     <row r="205" hidden="true">
       <c r="A205" t="s" s="2">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B205" s="2"/>
       <c r="C205" t="s" s="2">
@@ -25575,10 +25579,10 @@
         <v>71</v>
       </c>
       <c r="K205" t="s" s="2">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="L205" t="s" s="2">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="M205" s="2"/>
       <c r="N205" s="2"/>
@@ -25608,10 +25612,10 @@
         <v>185</v>
       </c>
       <c r="X205" t="s" s="2">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="Y205" t="s" s="2">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="Z205" t="s" s="2">
         <v>44</v>
@@ -25629,7 +25633,7 @@
         <v>44</v>
       </c>
       <c r="AE205" t="s" s="2">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="AF205" t="s" s="2">
         <v>52</v>
@@ -25644,7 +25648,7 @@
         <v>44</v>
       </c>
       <c r="AJ205" t="s" s="2">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="AK205" t="s" s="2">
         <v>114</v>

</xml_diff>

<commit_message>
Regenerated ACR,ES,PHR,PDL,SHS,SML Ig's after many narrative bugfixes and improvements to profile related pages.
</commit_message>
<xml_diff>
--- a/output/AdvanceCareRecords/patient-dh-base-1.xlsx
+++ b/output/AdvanceCareRecords/patient-dh-base-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7395" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7395" uniqueCount="648">
   <si>
     <t>Path</t>
   </si>
@@ -1439,10 +1439,6 @@
   </si>
   <si>
     <t>Patient.birthDate.value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-</t>
   </si>
   <si>
     <t>Primitive value for date</t>
@@ -20658,13 +20654,13 @@
         <v>44</v>
       </c>
       <c r="J162" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="K162" t="s" s="2">
         <v>447</v>
       </c>
-      <c r="K162" t="s" s="2">
+      <c r="L162" t="s" s="2">
         <v>448</v>
-      </c>
-      <c r="L162" t="s" s="2">
-        <v>449</v>
       </c>
       <c r="M162" s="2"/>
       <c r="N162" s="2"/>
@@ -20715,7 +20711,7 @@
         <v>44</v>
       </c>
       <c r="AE162" t="s" s="2">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AF162" t="s" s="2">
         <v>42</v>
@@ -20747,7 +20743,7 @@
     </row>
     <row r="163" hidden="true">
       <c r="A163" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" t="s" s="2">
@@ -20770,19 +20766,19 @@
         <v>53</v>
       </c>
       <c r="J163" t="s" s="2">
+        <v>451</v>
+      </c>
+      <c r="K163" t="s" s="2">
         <v>452</v>
       </c>
-      <c r="K163" t="s" s="2">
+      <c r="L163" t="s" s="2">
         <v>453</v>
       </c>
-      <c r="L163" t="s" s="2">
+      <c r="M163" t="s" s="2">
         <v>454</v>
       </c>
-      <c r="M163" t="s" s="2">
+      <c r="N163" t="s" s="2">
         <v>455</v>
-      </c>
-      <c r="N163" t="s" s="2">
-        <v>456</v>
       </c>
       <c r="O163" t="s" s="2">
         <v>44</v>
@@ -20829,7 +20825,7 @@
         <v>182</v>
       </c>
       <c r="AE163" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="AF163" t="s" s="2">
         <v>42</v>
@@ -20844,7 +20840,7 @@
         <v>44</v>
       </c>
       <c r="AJ163" t="s" s="2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AK163" t="s" s="2">
         <v>114</v>
@@ -20853,7 +20849,7 @@
         <v>44</v>
       </c>
       <c r="AM163" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="AN163" t="s" s="2">
         <v>44</v>
@@ -20861,10 +20857,10 @@
     </row>
     <row r="164">
       <c r="A164" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B164" t="s" s="2">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C164" t="s" s="2">
         <v>44</v>
@@ -20889,16 +20885,16 @@
         <v>381</v>
       </c>
       <c r="K164" t="s" s="2">
+        <v>459</v>
+      </c>
+      <c r="L164" t="s" s="2">
         <v>460</v>
       </c>
-      <c r="L164" t="s" s="2">
-        <v>461</v>
-      </c>
       <c r="M164" t="s" s="2">
+        <v>454</v>
+      </c>
+      <c r="N164" t="s" s="2">
         <v>455</v>
-      </c>
-      <c r="N164" t="s" s="2">
-        <v>456</v>
       </c>
       <c r="O164" t="s" s="2">
         <v>44</v>
@@ -20947,7 +20943,7 @@
         <v>44</v>
       </c>
       <c r="AE164" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="AF164" t="s" s="2">
         <v>42</v>
@@ -20962,7 +20958,7 @@
         <v>44</v>
       </c>
       <c r="AJ164" t="s" s="2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AK164" t="s" s="2">
         <v>114</v>
@@ -20971,7 +20967,7 @@
         <v>44</v>
       </c>
       <c r="AM164" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="AN164" t="s" s="2">
         <v>44</v>
@@ -20979,10 +20975,10 @@
     </row>
     <row r="165">
       <c r="A165" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B165" t="s" s="2">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C165" t="s" s="2">
         <v>44</v>
@@ -21007,16 +21003,16 @@
         <v>286</v>
       </c>
       <c r="K165" t="s" s="2">
+        <v>462</v>
+      </c>
+      <c r="L165" t="s" s="2">
         <v>463</v>
       </c>
-      <c r="L165" t="s" s="2">
-        <v>464</v>
-      </c>
       <c r="M165" t="s" s="2">
+        <v>454</v>
+      </c>
+      <c r="N165" t="s" s="2">
         <v>455</v>
-      </c>
-      <c r="N165" t="s" s="2">
-        <v>456</v>
       </c>
       <c r="O165" t="s" s="2">
         <v>44</v>
@@ -21065,7 +21061,7 @@
         <v>44</v>
       </c>
       <c r="AE165" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="AF165" t="s" s="2">
         <v>42</v>
@@ -21080,7 +21076,7 @@
         <v>44</v>
       </c>
       <c r="AJ165" t="s" s="2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AK165" t="s" s="2">
         <v>114</v>
@@ -21089,7 +21085,7 @@
         <v>44</v>
       </c>
       <c r="AM165" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="AN165" t="s" s="2">
         <v>44</v>
@@ -21097,7 +21093,7 @@
     </row>
     <row r="166" hidden="true">
       <c r="A166" t="s" s="2">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B166" s="2"/>
       <c r="C166" t="s" s="2">
@@ -21209,7 +21205,7 @@
     </row>
     <row r="167" hidden="true">
       <c r="A167" t="s" s="2">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B167" s="2"/>
       <c r="C167" t="s" s="2">
@@ -21319,7 +21315,7 @@
     </row>
     <row r="168">
       <c r="A168" t="s" s="2">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B168" t="s" s="2">
         <v>431</v>
@@ -21435,7 +21431,7 @@
     </row>
     <row r="169" hidden="true">
       <c r="A169" t="s" s="2">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B169" s="2"/>
       <c r="C169" t="s" s="2">
@@ -21458,13 +21454,13 @@
         <v>44</v>
       </c>
       <c r="J169" t="s" s="2">
-        <v>447</v>
+        <v>286</v>
       </c>
       <c r="K169" t="s" s="2">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="L169" t="s" s="2">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="M169" s="2"/>
       <c r="N169" s="2"/>
@@ -21515,7 +21511,7 @@
         <v>44</v>
       </c>
       <c r="AE169" t="s" s="2">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="AF169" t="s" s="2">
         <v>42</v>
@@ -21547,7 +21543,7 @@
     </row>
     <row r="170">
       <c r="A170" t="s" s="2">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B170" s="2"/>
       <c r="C170" t="s" s="2">
@@ -21573,16 +21569,16 @@
         <v>130</v>
       </c>
       <c r="K170" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="L170" t="s" s="2">
         <v>471</v>
       </c>
-      <c r="L170" t="s" s="2">
+      <c r="M170" t="s" s="2">
         <v>472</v>
       </c>
-      <c r="M170" t="s" s="2">
+      <c r="N170" t="s" s="2">
         <v>473</v>
-      </c>
-      <c r="N170" t="s" s="2">
-        <v>474</v>
       </c>
       <c r="O170" t="s" s="2">
         <v>44</v>
@@ -21631,7 +21627,7 @@
         <v>44</v>
       </c>
       <c r="AE170" t="s" s="2">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="AF170" t="s" s="2">
         <v>42</v>
@@ -21646,16 +21642,16 @@
         <v>44</v>
       </c>
       <c r="AJ170" t="s" s="2">
+        <v>474</v>
+      </c>
+      <c r="AK170" t="s" s="2">
         <v>475</v>
       </c>
-      <c r="AK170" t="s" s="2">
+      <c r="AL170" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM170" t="s" s="2">
         <v>476</v>
-      </c>
-      <c r="AL170" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM170" t="s" s="2">
-        <v>477</v>
       </c>
       <c r="AN170" t="s" s="2">
         <v>44</v>
@@ -21663,7 +21659,7 @@
     </row>
     <row r="171">
       <c r="A171" t="s" s="2">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B171" s="2"/>
       <c r="C171" t="s" s="2">
@@ -21689,14 +21685,14 @@
         <v>207</v>
       </c>
       <c r="K171" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="L171" t="s" s="2">
         <v>479</v>
-      </c>
-      <c r="L171" t="s" s="2">
-        <v>480</v>
       </c>
       <c r="M171" s="2"/>
       <c r="N171" t="s" s="2">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="O171" t="s" s="2">
         <v>44</v>
@@ -21724,52 +21720,52 @@
         <v>75</v>
       </c>
       <c r="X171" t="s" s="2">
+        <v>481</v>
+      </c>
+      <c r="Y171" t="s" s="2">
         <v>482</v>
       </c>
-      <c r="Y171" t="s" s="2">
+      <c r="Z171" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA171" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB171" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC171" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD171" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE171" t="s" s="2">
+        <v>477</v>
+      </c>
+      <c r="AF171" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG171" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH171" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI171" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ171" t="s" s="2">
         <v>483</v>
       </c>
-      <c r="Z171" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA171" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB171" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC171" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD171" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE171" t="s" s="2">
-        <v>478</v>
-      </c>
-      <c r="AF171" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG171" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH171" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI171" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ171" t="s" s="2">
+      <c r="AK171" t="s" s="2">
         <v>484</v>
       </c>
-      <c r="AK171" t="s" s="2">
+      <c r="AL171" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM171" t="s" s="2">
         <v>485</v>
-      </c>
-      <c r="AL171" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM171" t="s" s="2">
-        <v>486</v>
       </c>
       <c r="AN171" t="s" s="2">
         <v>44</v>
@@ -21777,7 +21773,7 @@
     </row>
     <row r="172">
       <c r="A172" t="s" s="2">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B172" s="2"/>
       <c r="C172" t="s" s="2">
@@ -21800,19 +21796,19 @@
         <v>44</v>
       </c>
       <c r="J172" t="s" s="2">
+        <v>487</v>
+      </c>
+      <c r="K172" t="s" s="2">
         <v>488</v>
       </c>
-      <c r="K172" t="s" s="2">
+      <c r="L172" t="s" s="2">
         <v>489</v>
       </c>
-      <c r="L172" t="s" s="2">
+      <c r="M172" t="s" s="2">
         <v>490</v>
       </c>
-      <c r="M172" t="s" s="2">
+      <c r="N172" t="s" s="2">
         <v>491</v>
-      </c>
-      <c r="N172" t="s" s="2">
-        <v>492</v>
       </c>
       <c r="O172" t="s" s="2">
         <v>44</v>
@@ -21861,7 +21857,7 @@
         <v>44</v>
       </c>
       <c r="AE172" t="s" s="2">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="AF172" t="s" s="2">
         <v>42</v>
@@ -21876,7 +21872,7 @@
         <v>44</v>
       </c>
       <c r="AJ172" t="s" s="2">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="AK172" t="s" s="2">
         <v>114</v>
@@ -21885,7 +21881,7 @@
         <v>44</v>
       </c>
       <c r="AM172" t="s" s="2">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="AN172" t="s" s="2">
         <v>44</v>
@@ -21893,7 +21889,7 @@
     </row>
     <row r="173" hidden="true">
       <c r="A173" t="s" s="2">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B173" s="2"/>
       <c r="C173" t="s" s="2">
@@ -21916,17 +21912,17 @@
         <v>44</v>
       </c>
       <c r="J173" t="s" s="2">
+        <v>495</v>
+      </c>
+      <c r="K173" t="s" s="2">
         <v>496</v>
       </c>
-      <c r="K173" t="s" s="2">
+      <c r="L173" t="s" s="2">
         <v>497</v>
-      </c>
-      <c r="L173" t="s" s="2">
-        <v>498</v>
       </c>
       <c r="M173" s="2"/>
       <c r="N173" t="s" s="2">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="O173" t="s" s="2">
         <v>44</v>
@@ -21975,7 +21971,7 @@
         <v>44</v>
       </c>
       <c r="AE173" t="s" s="2">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="AF173" t="s" s="2">
         <v>42</v>
@@ -21990,7 +21986,7 @@
         <v>44</v>
       </c>
       <c r="AJ173" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AK173" t="s" s="2">
         <v>114</v>
@@ -21999,7 +21995,7 @@
         <v>44</v>
       </c>
       <c r="AM173" t="s" s="2">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="AN173" t="s" s="2">
         <v>44</v>
@@ -22007,7 +22003,7 @@
     </row>
     <row r="174">
       <c r="A174" t="s" s="2">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B174" s="2"/>
       <c r="C174" t="s" s="2">
@@ -22030,19 +22026,19 @@
         <v>44</v>
       </c>
       <c r="J174" t="s" s="2">
+        <v>502</v>
+      </c>
+      <c r="K174" t="s" s="2">
         <v>503</v>
       </c>
-      <c r="K174" t="s" s="2">
+      <c r="L174" t="s" s="2">
         <v>504</v>
       </c>
-      <c r="L174" t="s" s="2">
+      <c r="M174" t="s" s="2">
         <v>505</v>
       </c>
-      <c r="M174" t="s" s="2">
+      <c r="N174" t="s" s="2">
         <v>506</v>
-      </c>
-      <c r="N174" t="s" s="2">
-        <v>507</v>
       </c>
       <c r="O174" t="s" s="2">
         <v>44</v>
@@ -22091,7 +22087,7 @@
         <v>44</v>
       </c>
       <c r="AE174" t="s" s="2">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AF174" t="s" s="2">
         <v>42</v>
@@ -22103,10 +22099,10 @@
         <v>44</v>
       </c>
       <c r="AI174" t="s" s="2">
+        <v>507</v>
+      </c>
+      <c r="AJ174" t="s" s="2">
         <v>508</v>
-      </c>
-      <c r="AJ174" t="s" s="2">
-        <v>509</v>
       </c>
       <c r="AK174" t="s" s="2">
         <v>114</v>
@@ -22123,7 +22119,7 @@
     </row>
     <row r="175" hidden="true">
       <c r="A175" t="s" s="2">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B175" s="2"/>
       <c r="C175" t="s" s="2">
@@ -22235,7 +22231,7 @@
     </row>
     <row r="176" hidden="true">
       <c r="A176" t="s" s="2">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B176" s="2"/>
       <c r="C176" t="s" s="2">
@@ -22349,11 +22345,11 @@
     </row>
     <row r="177" hidden="true">
       <c r="A177" t="s" s="2">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B177" s="2"/>
       <c r="C177" t="s" s="2">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D177" s="2"/>
       <c r="E177" t="s" s="2">
@@ -22378,7 +22374,7 @@
         <v>152</v>
       </c>
       <c r="L177" t="s" s="2">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="M177" t="s" s="2">
         <v>119</v>
@@ -22431,7 +22427,7 @@
         <v>44</v>
       </c>
       <c r="AE177" t="s" s="2">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AF177" t="s" s="2">
         <v>42</v>
@@ -22463,7 +22459,7 @@
     </row>
     <row r="178">
       <c r="A178" t="s" s="2">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B178" s="2"/>
       <c r="C178" t="s" s="2">
@@ -22489,14 +22485,14 @@
         <v>207</v>
       </c>
       <c r="K178" t="s" s="2">
+        <v>516</v>
+      </c>
+      <c r="L178" t="s" s="2">
         <v>517</v>
-      </c>
-      <c r="L178" t="s" s="2">
-        <v>518</v>
       </c>
       <c r="M178" s="2"/>
       <c r="N178" t="s" s="2">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="O178" t="s" s="2">
         <v>44</v>
@@ -22525,7 +22521,7 @@
       </c>
       <c r="X178" s="2"/>
       <c r="Y178" t="s" s="2">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="Z178" t="s" s="2">
         <v>44</v>
@@ -22543,7 +22539,7 @@
         <v>44</v>
       </c>
       <c r="AE178" t="s" s="2">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="AF178" t="s" s="2">
         <v>42</v>
@@ -22558,7 +22554,7 @@
         <v>44</v>
       </c>
       <c r="AJ178" t="s" s="2">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="AK178" t="s" s="2">
         <v>114</v>
@@ -22567,7 +22563,7 @@
         <v>44</v>
       </c>
       <c r="AM178" t="s" s="2">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="AN178" t="s" s="2">
         <v>44</v>
@@ -22575,7 +22571,7 @@
     </row>
     <row r="179">
       <c r="A179" t="s" s="2">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B179" s="2"/>
       <c r="C179" t="s" s="2">
@@ -22610,7 +22606,7 @@
         <v>393</v>
       </c>
       <c r="N179" t="s" s="2">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="O179" t="s" s="2">
         <v>44</v>
@@ -22659,7 +22655,7 @@
         <v>44</v>
       </c>
       <c r="AE179" t="s" s="2">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="AF179" t="s" s="2">
         <v>42</v>
@@ -22691,7 +22687,7 @@
     </row>
     <row r="180">
       <c r="A180" t="s" s="2">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B180" s="2"/>
       <c r="C180" t="s" s="2">
@@ -22717,13 +22713,13 @@
         <v>399</v>
       </c>
       <c r="K180" t="s" s="2">
+        <v>525</v>
+      </c>
+      <c r="L180" t="s" s="2">
         <v>526</v>
       </c>
-      <c r="L180" t="s" s="2">
+      <c r="M180" t="s" s="2">
         <v>527</v>
-      </c>
-      <c r="M180" t="s" s="2">
-        <v>528</v>
       </c>
       <c r="N180" t="s" s="2">
         <v>403</v>
@@ -22775,7 +22771,7 @@
         <v>44</v>
       </c>
       <c r="AE180" t="s" s="2">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="AF180" t="s" s="2">
         <v>42</v>
@@ -22799,7 +22795,7 @@
         <v>44</v>
       </c>
       <c r="AM180" t="s" s="2">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="AN180" t="s" s="2">
         <v>44</v>
@@ -22807,7 +22803,7 @@
     </row>
     <row r="181">
       <c r="A181" t="s" s="2">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B181" s="2"/>
       <c r="C181" t="s" s="2">
@@ -22833,14 +22829,14 @@
         <v>130</v>
       </c>
       <c r="K181" t="s" s="2">
+        <v>530</v>
+      </c>
+      <c r="L181" t="s" s="2">
         <v>531</v>
-      </c>
-      <c r="L181" t="s" s="2">
-        <v>532</v>
       </c>
       <c r="M181" s="2"/>
       <c r="N181" t="s" s="2">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="O181" t="s" s="2">
         <v>44</v>
@@ -22889,7 +22885,7 @@
         <v>44</v>
       </c>
       <c r="AE181" t="s" s="2">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AF181" t="s" s="2">
         <v>42</v>
@@ -22904,7 +22900,7 @@
         <v>44</v>
       </c>
       <c r="AJ181" t="s" s="2">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="AK181" t="s" s="2">
         <v>114</v>
@@ -22913,7 +22909,7 @@
         <v>44</v>
       </c>
       <c r="AM181" t="s" s="2">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="AN181" t="s" s="2">
         <v>44</v>
@@ -22921,7 +22917,7 @@
     </row>
     <row r="182">
       <c r="A182" t="s" s="2">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B182" s="2"/>
       <c r="C182" t="s" s="2">
@@ -22950,11 +22946,11 @@
         <v>408</v>
       </c>
       <c r="L182" t="s" s="2">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="M182" s="2"/>
       <c r="N182" t="s" s="2">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="O182" t="s" s="2">
         <v>44</v>
@@ -23003,7 +22999,7 @@
         <v>44</v>
       </c>
       <c r="AE182" t="s" s="2">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="AF182" t="s" s="2">
         <v>42</v>
@@ -23027,7 +23023,7 @@
         <v>44</v>
       </c>
       <c r="AM182" t="s" s="2">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AN182" t="s" s="2">
         <v>44</v>
@@ -23035,7 +23031,7 @@
     </row>
     <row r="183">
       <c r="A183" t="s" s="2">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B183" s="2"/>
       <c r="C183" t="s" s="2">
@@ -23058,17 +23054,17 @@
         <v>44</v>
       </c>
       <c r="J183" t="s" s="2">
+        <v>539</v>
+      </c>
+      <c r="K183" t="s" s="2">
         <v>540</v>
       </c>
-      <c r="K183" t="s" s="2">
+      <c r="L183" t="s" s="2">
         <v>541</v>
-      </c>
-      <c r="L183" t="s" s="2">
-        <v>542</v>
       </c>
       <c r="M183" s="2"/>
       <c r="N183" t="s" s="2">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="O183" t="s" s="2">
         <v>44</v>
@@ -23117,7 +23113,7 @@
         <v>44</v>
       </c>
       <c r="AE183" t="s" s="2">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AF183" t="s" s="2">
         <v>42</v>
@@ -23126,13 +23122,13 @@
         <v>52</v>
       </c>
       <c r="AH183" t="s" s="2">
+        <v>543</v>
+      </c>
+      <c r="AI183" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ183" t="s" s="2">
         <v>544</v>
-      </c>
-      <c r="AI183" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ183" t="s" s="2">
-        <v>545</v>
       </c>
       <c r="AK183" t="s" s="2">
         <v>114</v>
@@ -23141,7 +23137,7 @@
         <v>44</v>
       </c>
       <c r="AM183" t="s" s="2">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="AN183" t="s" s="2">
         <v>44</v>
@@ -23149,7 +23145,7 @@
     </row>
     <row r="184">
       <c r="A184" t="s" s="2">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B184" s="2"/>
       <c r="C184" t="s" s="2">
@@ -23175,10 +23171,10 @@
         <v>255</v>
       </c>
       <c r="K184" t="s" s="2">
+        <v>547</v>
+      </c>
+      <c r="L184" t="s" s="2">
         <v>548</v>
-      </c>
-      <c r="L184" t="s" s="2">
-        <v>549</v>
       </c>
       <c r="M184" s="2"/>
       <c r="N184" s="2"/>
@@ -23229,7 +23225,7 @@
         <v>44</v>
       </c>
       <c r="AE184" t="s" s="2">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AF184" t="s" s="2">
         <v>42</v>
@@ -23244,7 +23240,7 @@
         <v>44</v>
       </c>
       <c r="AJ184" t="s" s="2">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AK184" t="s" s="2">
         <v>114</v>
@@ -23261,7 +23257,7 @@
     </row>
     <row r="185" hidden="true">
       <c r="A185" t="s" s="2">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B185" s="2"/>
       <c r="C185" t="s" s="2">
@@ -23284,19 +23280,19 @@
         <v>53</v>
       </c>
       <c r="J185" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K185" t="s" s="2">
+        <v>551</v>
+      </c>
+      <c r="L185" t="s" s="2">
         <v>552</v>
       </c>
-      <c r="L185" t="s" s="2">
+      <c r="M185" t="s" s="2">
         <v>553</v>
       </c>
-      <c r="M185" t="s" s="2">
+      <c r="N185" t="s" s="2">
         <v>554</v>
-      </c>
-      <c r="N185" t="s" s="2">
-        <v>555</v>
       </c>
       <c r="O185" t="s" s="2">
         <v>44</v>
@@ -23345,7 +23341,7 @@
         <v>44</v>
       </c>
       <c r="AE185" t="s" s="2">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="AF185" t="s" s="2">
         <v>42</v>
@@ -23357,10 +23353,10 @@
         <v>44</v>
       </c>
       <c r="AI185" t="s" s="2">
+        <v>555</v>
+      </c>
+      <c r="AJ185" t="s" s="2">
         <v>556</v>
-      </c>
-      <c r="AJ185" t="s" s="2">
-        <v>557</v>
       </c>
       <c r="AK185" t="s" s="2">
         <v>114</v>
@@ -23377,7 +23373,7 @@
     </row>
     <row r="186" hidden="true">
       <c r="A186" t="s" s="2">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B186" s="2"/>
       <c r="C186" t="s" s="2">
@@ -23489,7 +23485,7 @@
     </row>
     <row r="187" hidden="true">
       <c r="A187" t="s" s="2">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B187" s="2"/>
       <c r="C187" t="s" s="2">
@@ -23603,11 +23599,11 @@
     </row>
     <row r="188" hidden="true">
       <c r="A188" t="s" s="2">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B188" s="2"/>
       <c r="C188" t="s" s="2">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D188" s="2"/>
       <c r="E188" t="s" s="2">
@@ -23632,7 +23628,7 @@
         <v>152</v>
       </c>
       <c r="L188" t="s" s="2">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="M188" t="s" s="2">
         <v>119</v>
@@ -23685,7 +23681,7 @@
         <v>44</v>
       </c>
       <c r="AE188" t="s" s="2">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AF188" t="s" s="2">
         <v>42</v>
@@ -23717,7 +23713,7 @@
     </row>
     <row r="189" hidden="true">
       <c r="A189" t="s" s="2">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B189" s="2"/>
       <c r="C189" t="s" s="2">
@@ -23743,16 +23739,16 @@
         <v>207</v>
       </c>
       <c r="K189" t="s" s="2">
+        <v>561</v>
+      </c>
+      <c r="L189" t="s" s="2">
         <v>562</v>
       </c>
-      <c r="L189" t="s" s="2">
+      <c r="M189" t="s" s="2">
         <v>563</v>
       </c>
-      <c r="M189" t="s" s="2">
+      <c r="N189" t="s" s="2">
         <v>564</v>
-      </c>
-      <c r="N189" t="s" s="2">
-        <v>565</v>
       </c>
       <c r="O189" t="s" s="2">
         <v>44</v>
@@ -23777,14 +23773,14 @@
         <v>44</v>
       </c>
       <c r="W189" t="s" s="2">
+        <v>565</v>
+      </c>
+      <c r="X189" t="s" s="2">
         <v>566</v>
       </c>
-      <c r="X189" t="s" s="2">
+      <c r="Y189" t="s" s="2">
         <v>567</v>
       </c>
-      <c r="Y189" t="s" s="2">
-        <v>568</v>
-      </c>
       <c r="Z189" t="s" s="2">
         <v>44</v>
       </c>
@@ -23801,7 +23797,7 @@
         <v>44</v>
       </c>
       <c r="AE189" t="s" s="2">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="AF189" t="s" s="2">
         <v>52</v>
@@ -23816,7 +23812,7 @@
         <v>44</v>
       </c>
       <c r="AJ189" t="s" s="2">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="AK189" t="s" s="2">
         <v>114</v>
@@ -23825,7 +23821,7 @@
         <v>44</v>
       </c>
       <c r="AM189" t="s" s="2">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="AN189" t="s" s="2">
         <v>44</v>
@@ -23833,7 +23829,7 @@
     </row>
     <row r="190" hidden="true">
       <c r="A190" t="s" s="2">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B190" s="2"/>
       <c r="C190" t="s" s="2">
@@ -23859,16 +23855,16 @@
         <v>207</v>
       </c>
       <c r="K190" t="s" s="2">
+        <v>570</v>
+      </c>
+      <c r="L190" t="s" s="2">
         <v>571</v>
       </c>
-      <c r="L190" t="s" s="2">
+      <c r="M190" t="s" s="2">
         <v>572</v>
       </c>
-      <c r="M190" t="s" s="2">
+      <c r="N190" t="s" s="2">
         <v>573</v>
-      </c>
-      <c r="N190" t="s" s="2">
-        <v>574</v>
       </c>
       <c r="O190" t="s" s="2">
         <v>44</v>
@@ -23893,46 +23889,46 @@
         <v>44</v>
       </c>
       <c r="W190" t="s" s="2">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="X190" t="s" s="2">
+        <v>574</v>
+      </c>
+      <c r="Y190" t="s" s="2">
         <v>575</v>
       </c>
-      <c r="Y190" t="s" s="2">
+      <c r="Z190" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA190" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB190" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC190" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD190" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE190" t="s" s="2">
+        <v>569</v>
+      </c>
+      <c r="AF190" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG190" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH190" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI190" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ190" t="s" s="2">
         <v>576</v>
-      </c>
-      <c r="Z190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE190" t="s" s="2">
-        <v>570</v>
-      </c>
-      <c r="AF190" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG190" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ190" t="s" s="2">
-        <v>577</v>
       </c>
       <c r="AK190" t="s" s="2">
         <v>114</v>
@@ -23941,7 +23937,7 @@
         <v>44</v>
       </c>
       <c r="AM190" t="s" s="2">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="AN190" t="s" s="2">
         <v>44</v>
@@ -23949,7 +23945,7 @@
     </row>
     <row r="191" hidden="true">
       <c r="A191" t="s" s="2">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B191" s="2"/>
       <c r="C191" t="s" s="2">
@@ -23975,14 +23971,14 @@
         <v>207</v>
       </c>
       <c r="K191" t="s" s="2">
+        <v>579</v>
+      </c>
+      <c r="L191" t="s" s="2">
         <v>580</v>
-      </c>
-      <c r="L191" t="s" s="2">
-        <v>581</v>
       </c>
       <c r="M191" s="2"/>
       <c r="N191" t="s" s="2">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="O191" t="s" s="2">
         <v>44</v>
@@ -24007,46 +24003,46 @@
         <v>44</v>
       </c>
       <c r="W191" t="s" s="2">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="X191" t="s" s="2">
+        <v>582</v>
+      </c>
+      <c r="Y191" t="s" s="2">
         <v>583</v>
       </c>
-      <c r="Y191" t="s" s="2">
+      <c r="Z191" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA191" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB191" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC191" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD191" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE191" t="s" s="2">
+        <v>578</v>
+      </c>
+      <c r="AF191" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG191" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH191" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI191" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ191" t="s" s="2">
         <v>584</v>
-      </c>
-      <c r="Z191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE191" t="s" s="2">
-        <v>579</v>
-      </c>
-      <c r="AF191" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG191" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ191" t="s" s="2">
-        <v>585</v>
       </c>
       <c r="AK191" t="s" s="2">
         <v>114</v>
@@ -24063,7 +24059,7 @@
     </row>
     <row r="192">
       <c r="A192" t="s" s="2">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B192" s="2"/>
       <c r="C192" t="s" s="2">
@@ -24086,19 +24082,19 @@
         <v>44</v>
       </c>
       <c r="J192" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K192" t="s" s="2">
+        <v>586</v>
+      </c>
+      <c r="L192" t="s" s="2">
         <v>587</v>
       </c>
-      <c r="L192" t="s" s="2">
+      <c r="M192" t="s" s="2">
         <v>588</v>
       </c>
-      <c r="M192" t="s" s="2">
+      <c r="N192" t="s" s="2">
         <v>589</v>
-      </c>
-      <c r="N192" t="s" s="2">
-        <v>590</v>
       </c>
       <c r="O192" t="s" s="2">
         <v>44</v>
@@ -24147,7 +24143,7 @@
         <v>44</v>
       </c>
       <c r="AE192" t="s" s="2">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="AF192" t="s" s="2">
         <v>42</v>
@@ -24159,13 +24155,13 @@
         <v>44</v>
       </c>
       <c r="AI192" t="s" s="2">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AJ192" t="s" s="2">
+        <v>590</v>
+      </c>
+      <c r="AK192" t="s" s="2">
         <v>591</v>
-      </c>
-      <c r="AK192" t="s" s="2">
-        <v>592</v>
       </c>
       <c r="AL192" t="s" s="2">
         <v>44</v>
@@ -24179,7 +24175,7 @@
     </row>
     <row r="193" hidden="true">
       <c r="A193" t="s" s="2">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B193" s="2"/>
       <c r="C193" t="s" s="2">
@@ -24291,7 +24287,7 @@
     </row>
     <row r="194" hidden="true">
       <c r="A194" t="s" s="2">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B194" s="2"/>
       <c r="C194" t="s" s="2">
@@ -24405,11 +24401,11 @@
     </row>
     <row r="195" hidden="true">
       <c r="A195" t="s" s="2">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B195" s="2"/>
       <c r="C195" t="s" s="2">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D195" s="2"/>
       <c r="E195" t="s" s="2">
@@ -24434,7 +24430,7 @@
         <v>152</v>
       </c>
       <c r="L195" t="s" s="2">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="M195" t="s" s="2">
         <v>119</v>
@@ -24487,7 +24483,7 @@
         <v>44</v>
       </c>
       <c r="AE195" t="s" s="2">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AF195" t="s" s="2">
         <v>42</v>
@@ -24519,7 +24515,7 @@
     </row>
     <row r="196">
       <c r="A196" t="s" s="2">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B196" s="2"/>
       <c r="C196" t="s" s="2">
@@ -24545,16 +24541,16 @@
         <v>207</v>
       </c>
       <c r="K196" t="s" s="2">
+        <v>596</v>
+      </c>
+      <c r="L196" t="s" s="2">
         <v>597</v>
       </c>
-      <c r="L196" t="s" s="2">
+      <c r="M196" t="s" s="2">
         <v>598</v>
       </c>
-      <c r="M196" t="s" s="2">
+      <c r="N196" t="s" s="2">
         <v>599</v>
-      </c>
-      <c r="N196" t="s" s="2">
-        <v>600</v>
       </c>
       <c r="O196" t="s" s="2">
         <v>44</v>
@@ -24583,49 +24579,49 @@
       </c>
       <c r="X196" s="2"/>
       <c r="Y196" t="s" s="2">
+        <v>600</v>
+      </c>
+      <c r="Z196" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA196" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB196" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC196" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD196" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE196" t="s" s="2">
+        <v>595</v>
+      </c>
+      <c r="AF196" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AG196" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH196" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI196" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ196" t="s" s="2">
         <v>601</v>
       </c>
-      <c r="Z196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE196" t="s" s="2">
-        <v>596</v>
-      </c>
-      <c r="AF196" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AG196" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ196" t="s" s="2">
+      <c r="AK196" t="s" s="2">
         <v>602</v>
       </c>
-      <c r="AK196" t="s" s="2">
+      <c r="AL196" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM196" t="s" s="2">
         <v>603</v>
-      </c>
-      <c r="AL196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM196" t="s" s="2">
-        <v>604</v>
       </c>
       <c r="AN196" t="s" s="2">
         <v>44</v>
@@ -24633,7 +24629,7 @@
     </row>
     <row r="197">
       <c r="A197" t="s" s="2">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B197" s="2"/>
       <c r="C197" t="s" s="2">
@@ -24659,16 +24655,16 @@
         <v>381</v>
       </c>
       <c r="K197" t="s" s="2">
+        <v>605</v>
+      </c>
+      <c r="L197" t="s" s="2">
         <v>606</v>
       </c>
-      <c r="L197" t="s" s="2">
+      <c r="M197" t="s" s="2">
         <v>607</v>
       </c>
-      <c r="M197" t="s" s="2">
+      <c r="N197" t="s" s="2">
         <v>608</v>
-      </c>
-      <c r="N197" t="s" s="2">
-        <v>609</v>
       </c>
       <c r="O197" t="s" s="2">
         <v>44</v>
@@ -24717,7 +24713,7 @@
         <v>44</v>
       </c>
       <c r="AE197" t="s" s="2">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AF197" t="s" s="2">
         <v>42</v>
@@ -24732,16 +24728,16 @@
         <v>44</v>
       </c>
       <c r="AJ197" t="s" s="2">
+        <v>609</v>
+      </c>
+      <c r="AK197" t="s" s="2">
         <v>610</v>
       </c>
-      <c r="AK197" t="s" s="2">
+      <c r="AL197" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM197" t="s" s="2">
         <v>611</v>
-      </c>
-      <c r="AL197" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM197" t="s" s="2">
-        <v>612</v>
       </c>
       <c r="AN197" t="s" s="2">
         <v>44</v>
@@ -24749,14 +24745,14 @@
     </row>
     <row r="198">
       <c r="A198" t="s" s="2">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B198" s="2"/>
       <c r="C198" t="s" s="2">
+        <v>613</v>
+      </c>
+      <c r="D198" t="s" s="2">
         <v>614</v>
-      </c>
-      <c r="D198" t="s" s="2">
-        <v>615</v>
       </c>
       <c r="E198" t="s" s="2">
         <v>42</v>
@@ -24774,16 +24770,16 @@
         <v>44</v>
       </c>
       <c r="J198" t="s" s="2">
+        <v>615</v>
+      </c>
+      <c r="K198" t="s" s="2">
         <v>616</v>
       </c>
-      <c r="K198" t="s" s="2">
+      <c r="L198" t="s" s="2">
         <v>617</v>
       </c>
-      <c r="L198" t="s" s="2">
+      <c r="M198" t="s" s="2">
         <v>618</v>
-      </c>
-      <c r="M198" t="s" s="2">
-        <v>619</v>
       </c>
       <c r="N198" s="2"/>
       <c r="O198" t="s" s="2">
@@ -24833,7 +24829,7 @@
         <v>44</v>
       </c>
       <c r="AE198" t="s" s="2">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AF198" t="s" s="2">
         <v>42</v>
@@ -24848,7 +24844,7 @@
         <v>44</v>
       </c>
       <c r="AJ198" t="s" s="2">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="AK198" t="s" s="2">
         <v>114</v>
@@ -24857,7 +24853,7 @@
         <v>44</v>
       </c>
       <c r="AM198" t="s" s="2">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AN198" t="s" s="2">
         <v>44</v>
@@ -24865,14 +24861,14 @@
     </row>
     <row r="199">
       <c r="A199" t="s" s="2">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B199" s="2"/>
       <c r="C199" t="s" s="2">
         <v>44</v>
       </c>
       <c r="D199" t="s" s="2">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E199" t="s" s="2">
         <v>42</v>
@@ -24890,19 +24886,19 @@
         <v>53</v>
       </c>
       <c r="J199" t="s" s="2">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K199" t="s" s="2">
+        <v>623</v>
+      </c>
+      <c r="L199" t="s" s="2">
         <v>624</v>
       </c>
-      <c r="L199" t="s" s="2">
+      <c r="M199" t="s" s="2">
         <v>625</v>
       </c>
-      <c r="M199" t="s" s="2">
+      <c r="N199" t="s" s="2">
         <v>626</v>
-      </c>
-      <c r="N199" t="s" s="2">
-        <v>627</v>
       </c>
       <c r="O199" t="s" s="2">
         <v>44</v>
@@ -24951,7 +24947,7 @@
         <v>44</v>
       </c>
       <c r="AE199" t="s" s="2">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="AF199" t="s" s="2">
         <v>42</v>
@@ -24966,10 +24962,10 @@
         <v>44</v>
       </c>
       <c r="AJ199" t="s" s="2">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="AK199" t="s" s="2">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="AL199" t="s" s="2">
         <v>44</v>
@@ -24983,7 +24979,7 @@
     </row>
     <row r="200" hidden="true">
       <c r="A200" t="s" s="2">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B200" s="2"/>
       <c r="C200" t="s" s="2">
@@ -25006,19 +25002,19 @@
         <v>53</v>
       </c>
       <c r="J200" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K200" t="s" s="2">
+        <v>629</v>
+      </c>
+      <c r="L200" t="s" s="2">
         <v>630</v>
       </c>
-      <c r="L200" t="s" s="2">
+      <c r="M200" t="s" s="2">
         <v>631</v>
       </c>
-      <c r="M200" t="s" s="2">
+      <c r="N200" t="s" s="2">
         <v>632</v>
-      </c>
-      <c r="N200" t="s" s="2">
-        <v>633</v>
       </c>
       <c r="O200" t="s" s="2">
         <v>44</v>
@@ -25067,7 +25063,7 @@
         <v>44</v>
       </c>
       <c r="AE200" t="s" s="2">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AF200" t="s" s="2">
         <v>42</v>
@@ -25079,10 +25075,10 @@
         <v>44</v>
       </c>
       <c r="AI200" t="s" s="2">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AJ200" t="s" s="2">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="AK200" t="s" s="2">
         <v>114</v>
@@ -25099,7 +25095,7 @@
     </row>
     <row r="201" hidden="true">
       <c r="A201" t="s" s="2">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B201" s="2"/>
       <c r="C201" t="s" s="2">
@@ -25211,7 +25207,7 @@
     </row>
     <row r="202" hidden="true">
       <c r="A202" t="s" s="2">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B202" s="2"/>
       <c r="C202" t="s" s="2">
@@ -25325,11 +25321,11 @@
     </row>
     <row r="203" hidden="true">
       <c r="A203" t="s" s="2">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B203" s="2"/>
       <c r="C203" t="s" s="2">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D203" s="2"/>
       <c r="E203" t="s" s="2">
@@ -25354,7 +25350,7 @@
         <v>152</v>
       </c>
       <c r="L203" t="s" s="2">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="M203" t="s" s="2">
         <v>119</v>
@@ -25407,7 +25403,7 @@
         <v>44</v>
       </c>
       <c r="AE203" t="s" s="2">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AF203" t="s" s="2">
         <v>42</v>
@@ -25439,7 +25435,7 @@
     </row>
     <row r="204" hidden="true">
       <c r="A204" t="s" s="2">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B204" s="2"/>
       <c r="C204" t="s" s="2">
@@ -25462,16 +25458,16 @@
         <v>53</v>
       </c>
       <c r="J204" t="s" s="2">
+        <v>638</v>
+      </c>
+      <c r="K204" t="s" s="2">
         <v>639</v>
       </c>
-      <c r="K204" t="s" s="2">
+      <c r="L204" t="s" s="2">
         <v>640</v>
       </c>
-      <c r="L204" t="s" s="2">
+      <c r="M204" t="s" s="2">
         <v>641</v>
-      </c>
-      <c r="M204" t="s" s="2">
-        <v>642</v>
       </c>
       <c r="N204" s="2"/>
       <c r="O204" t="s" s="2">
@@ -25521,7 +25517,7 @@
         <v>44</v>
       </c>
       <c r="AE204" t="s" s="2">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="AF204" t="s" s="2">
         <v>52</v>
@@ -25545,7 +25541,7 @@
         <v>44</v>
       </c>
       <c r="AM204" t="s" s="2">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AN204" t="s" s="2">
         <v>44</v>
@@ -25553,7 +25549,7 @@
     </row>
     <row r="205" hidden="true">
       <c r="A205" t="s" s="2">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B205" s="2"/>
       <c r="C205" t="s" s="2">
@@ -25579,10 +25575,10 @@
         <v>71</v>
       </c>
       <c r="K205" t="s" s="2">
+        <v>644</v>
+      </c>
+      <c r="L205" t="s" s="2">
         <v>645</v>
-      </c>
-      <c r="L205" t="s" s="2">
-        <v>646</v>
       </c>
       <c r="M205" s="2"/>
       <c r="N205" s="2"/>
@@ -25612,43 +25608,43 @@
         <v>185</v>
       </c>
       <c r="X205" t="s" s="2">
+        <v>645</v>
+      </c>
+      <c r="Y205" t="s" s="2">
         <v>646</v>
       </c>
-      <c r="Y205" t="s" s="2">
+      <c r="Z205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE205" t="s" s="2">
+        <v>643</v>
+      </c>
+      <c r="AF205" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AG205" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ205" t="s" s="2">
         <v>647</v>
-      </c>
-      <c r="Z205" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA205" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB205" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC205" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD205" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE205" t="s" s="2">
-        <v>644</v>
-      </c>
-      <c r="AF205" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AG205" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH205" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI205" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ205" t="s" s="2">
-        <v>648</v>
       </c>
       <c r="AK205" t="s" s="2">
         <v>114</v>

</xml_diff>